<commit_message>
Added web form metadata to type configs
</commit_message>
<xml_diff>
--- a/SolutionItems/Customisations.xlsx
+++ b/SolutionItems/Customisations.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="23820" windowHeight="8010"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="23820" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Record Types" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="149">
   <si>
     <t>Relationship Name</t>
   </si>
@@ -409,6 +409,66 @@
   </si>
   <si>
     <t>Entity Form Metadata</t>
+  </si>
+  <si>
+    <t>Web Form</t>
+  </si>
+  <si>
+    <t>adx_webform</t>
+  </si>
+  <si>
+    <t>Web Forms</t>
+  </si>
+  <si>
+    <t>Defines the necessary properties and relationships to the other key entities in order to control the initialization of the form within a web portal.</t>
+  </si>
+  <si>
+    <t>Web Form Metadata</t>
+  </si>
+  <si>
+    <t>adx_webformmetadata</t>
+  </si>
+  <si>
+    <t>Defines the additional behavior modification logic to augment or override the functionality of form fields that is not possible with entity and form metadata.</t>
+  </si>
+  <si>
+    <t>Web Form Step</t>
+  </si>
+  <si>
+    <t>adx_webformstep</t>
+  </si>
+  <si>
+    <t>Web Form Steps</t>
+  </si>
+  <si>
+    <t>Defines the flow logic of the form's user experience such as steps and conditional branching.</t>
+  </si>
+  <si>
+    <t>Type the name of the custom entity.</t>
+  </si>
+  <si>
+    <t>Unique identifier for Web Form associated with Web Form Step.</t>
+  </si>
+  <si>
+    <t>Attribute Logical Name</t>
+  </si>
+  <si>
+    <t>The name of the attribute field to be modified</t>
+  </si>
+  <si>
+    <t>Unique identifier for Web Form Step associated with Web Form Metadata.</t>
+  </si>
+  <si>
+    <t>Purchase</t>
+  </si>
+  <si>
+    <t>WebFormMtType</t>
+  </si>
+  <si>
+    <t>Tab Name</t>
+  </si>
+  <si>
+    <t>Subgrid Name</t>
   </si>
 </sst>
 </file>
@@ -768,10 +828,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1168,6 +1228,111 @@
         <v>0</v>
       </c>
     </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>129</v>
+      </c>
+      <c r="B12" t="s">
+        <v>130</v>
+      </c>
+      <c r="C12" t="s">
+        <v>131</v>
+      </c>
+      <c r="D12" t="s">
+        <v>132</v>
+      </c>
+      <c r="E12" t="b">
+        <v>0</v>
+      </c>
+      <c r="F12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G12" t="b">
+        <v>0</v>
+      </c>
+      <c r="H12" t="b">
+        <v>0</v>
+      </c>
+      <c r="I12" t="b">
+        <v>0</v>
+      </c>
+      <c r="J12" t="b">
+        <v>0</v>
+      </c>
+      <c r="K12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>133</v>
+      </c>
+      <c r="B13" t="s">
+        <v>134</v>
+      </c>
+      <c r="C13" t="s">
+        <v>133</v>
+      </c>
+      <c r="D13" t="s">
+        <v>135</v>
+      </c>
+      <c r="E13" t="b">
+        <v>0</v>
+      </c>
+      <c r="F13" t="b">
+        <v>0</v>
+      </c>
+      <c r="G13" t="b">
+        <v>0</v>
+      </c>
+      <c r="H13" t="b">
+        <v>0</v>
+      </c>
+      <c r="I13" t="b">
+        <v>0</v>
+      </c>
+      <c r="J13" t="b">
+        <v>0</v>
+      </c>
+      <c r="K13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>136</v>
+      </c>
+      <c r="B14" t="s">
+        <v>137</v>
+      </c>
+      <c r="C14" t="s">
+        <v>138</v>
+      </c>
+      <c r="D14" t="s">
+        <v>139</v>
+      </c>
+      <c r="E14" t="b">
+        <v>0</v>
+      </c>
+      <c r="F14" t="b">
+        <v>0</v>
+      </c>
+      <c r="G14" t="b">
+        <v>0</v>
+      </c>
+      <c r="H14" t="b">
+        <v>0</v>
+      </c>
+      <c r="I14" t="b">
+        <v>0</v>
+      </c>
+      <c r="J14" t="b">
+        <v>0</v>
+      </c>
+      <c r="K14" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1176,10 +1341,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X35"/>
+  <dimension ref="A1:T44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView topLeftCell="N7" workbookViewId="0">
+      <selection activeCell="T33" sqref="T33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2192,7 +2357,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>80</v>
       </c>
@@ -2254,7 +2419,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>81</v>
       </c>
@@ -2316,7 +2481,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>81</v>
       </c>
@@ -2378,7 +2543,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:24" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>92</v>
       </c>
@@ -2435,12 +2600,8 @@
       <c r="T20" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="U20" s="4"/>
-      <c r="V20" s="4"/>
-      <c r="W20" s="4"/>
-      <c r="X20" s="4"/>
-    </row>
-    <row r="21" spans="1:24" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:20" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>94</v>
       </c>
@@ -2497,12 +2658,8 @@
       <c r="T21" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="U21" s="4"/>
-      <c r="V21" s="4"/>
-      <c r="W21" s="4"/>
-      <c r="X21" s="4"/>
-    </row>
-    <row r="22" spans="1:24" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:20" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>95</v>
       </c>
@@ -2559,12 +2716,8 @@
       <c r="T22" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="U22" s="4"/>
-      <c r="V22" s="4"/>
-      <c r="W22" s="4"/>
-      <c r="X22" s="4"/>
-    </row>
-    <row r="23" spans="1:24" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:20" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>96</v>
       </c>
@@ -2621,12 +2774,8 @@
       <c r="T23" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="U23" s="4"/>
-      <c r="V23" s="4"/>
-      <c r="W23" s="4"/>
-      <c r="X23" s="4"/>
-    </row>
-    <row r="24" spans="1:24" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:20" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>97</v>
       </c>
@@ -2683,12 +2832,8 @@
       <c r="T24" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="U24" s="4"/>
-      <c r="V24" s="4"/>
-      <c r="W24" s="4"/>
-      <c r="X24" s="4"/>
-    </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>94</v>
       </c>
@@ -2750,7 +2895,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>94</v>
       </c>
@@ -2812,7 +2957,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>97</v>
       </c>
@@ -2874,7 +3019,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:24" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>105</v>
       </c>
@@ -2931,12 +3076,8 @@
       <c r="T28" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="U28" s="4"/>
-      <c r="V28" s="4"/>
-      <c r="W28" s="4"/>
-      <c r="X28" s="4"/>
-    </row>
-    <row r="29" spans="1:24" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:20" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>106</v>
       </c>
@@ -2993,12 +3134,8 @@
       <c r="T29" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="U29" s="4"/>
-      <c r="V29" s="4"/>
-      <c r="W29" s="4"/>
-      <c r="X29" s="4"/>
-    </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>106</v>
       </c>
@@ -3060,7 +3197,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>106</v>
       </c>
@@ -3122,7 +3259,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>106</v>
       </c>
@@ -3368,6 +3505,462 @@
       </c>
       <c r="T35" s="1" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>130</v>
+      </c>
+      <c r="B36" t="s">
+        <v>93</v>
+      </c>
+      <c r="C36" t="s">
+        <v>12</v>
+      </c>
+      <c r="D36" t="s">
+        <v>1</v>
+      </c>
+      <c r="E36" t="s">
+        <v>140</v>
+      </c>
+      <c r="F36" t="b">
+        <v>1</v>
+      </c>
+      <c r="G36" t="b">
+        <v>1</v>
+      </c>
+      <c r="H36" t="b">
+        <v>1</v>
+      </c>
+      <c r="I36" t="b">
+        <v>1</v>
+      </c>
+      <c r="L36" t="s">
+        <v>29</v>
+      </c>
+      <c r="M36" t="b">
+        <v>0</v>
+      </c>
+      <c r="N36">
+        <v>100</v>
+      </c>
+      <c r="O36" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>29</v>
+      </c>
+      <c r="R36" t="b">
+        <v>0</v>
+      </c>
+      <c r="S36">
+        <v>-1</v>
+      </c>
+      <c r="T36" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>137</v>
+      </c>
+      <c r="B37" t="s">
+        <v>93</v>
+      </c>
+      <c r="C37" t="s">
+        <v>12</v>
+      </c>
+      <c r="D37" t="s">
+        <v>1</v>
+      </c>
+      <c r="E37" t="s">
+        <v>140</v>
+      </c>
+      <c r="F37" t="b">
+        <v>1</v>
+      </c>
+      <c r="G37" t="b">
+        <v>1</v>
+      </c>
+      <c r="H37" t="b">
+        <v>1</v>
+      </c>
+      <c r="I37" t="b">
+        <v>1</v>
+      </c>
+      <c r="L37" t="s">
+        <v>29</v>
+      </c>
+      <c r="M37" t="b">
+        <v>0</v>
+      </c>
+      <c r="N37">
+        <v>100</v>
+      </c>
+      <c r="O37" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q37" t="s">
+        <v>29</v>
+      </c>
+      <c r="R37" t="b">
+        <v>0</v>
+      </c>
+      <c r="S37">
+        <v>-1</v>
+      </c>
+      <c r="T37" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>137</v>
+      </c>
+      <c r="B38" t="s">
+        <v>130</v>
+      </c>
+      <c r="C38" t="s">
+        <v>129</v>
+      </c>
+      <c r="D38" t="s">
+        <v>59</v>
+      </c>
+      <c r="E38" t="s">
+        <v>141</v>
+      </c>
+      <c r="F38" t="b">
+        <v>0</v>
+      </c>
+      <c r="G38" t="b">
+        <v>1</v>
+      </c>
+      <c r="H38" t="b">
+        <v>0</v>
+      </c>
+      <c r="I38" t="b">
+        <v>1</v>
+      </c>
+      <c r="L38" t="s">
+        <v>130</v>
+      </c>
+      <c r="M38" t="b">
+        <v>1</v>
+      </c>
+      <c r="N38">
+        <v>-1</v>
+      </c>
+      <c r="Q38" t="s">
+        <v>29</v>
+      </c>
+      <c r="R38" t="b">
+        <v>0</v>
+      </c>
+      <c r="S38">
+        <v>-1</v>
+      </c>
+      <c r="T38" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>134</v>
+      </c>
+      <c r="B39" t="s">
+        <v>109</v>
+      </c>
+      <c r="C39" t="s">
+        <v>142</v>
+      </c>
+      <c r="D39" t="s">
+        <v>1</v>
+      </c>
+      <c r="E39" t="s">
+        <v>143</v>
+      </c>
+      <c r="F39" t="b">
+        <v>1</v>
+      </c>
+      <c r="G39" t="b">
+        <v>0</v>
+      </c>
+      <c r="H39" t="b">
+        <v>1</v>
+      </c>
+      <c r="I39" t="b">
+        <v>1</v>
+      </c>
+      <c r="L39" t="s">
+        <v>29</v>
+      </c>
+      <c r="M39" t="b">
+        <v>0</v>
+      </c>
+      <c r="N39">
+        <v>100</v>
+      </c>
+      <c r="O39" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q39" t="s">
+        <v>29</v>
+      </c>
+      <c r="R39" t="b">
+        <v>0</v>
+      </c>
+      <c r="S39">
+        <v>-1</v>
+      </c>
+      <c r="T39" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>134</v>
+      </c>
+      <c r="B40" t="s">
+        <v>137</v>
+      </c>
+      <c r="C40" t="s">
+        <v>136</v>
+      </c>
+      <c r="D40" t="s">
+        <v>59</v>
+      </c>
+      <c r="E40" t="s">
+        <v>144</v>
+      </c>
+      <c r="F40" t="b">
+        <v>0</v>
+      </c>
+      <c r="G40" t="b">
+        <v>1</v>
+      </c>
+      <c r="H40" t="b">
+        <v>0</v>
+      </c>
+      <c r="I40" t="b">
+        <v>1</v>
+      </c>
+      <c r="L40" t="s">
+        <v>137</v>
+      </c>
+      <c r="M40" t="b">
+        <v>1</v>
+      </c>
+      <c r="N40">
+        <v>-1</v>
+      </c>
+      <c r="Q40" t="s">
+        <v>29</v>
+      </c>
+      <c r="R40" t="b">
+        <v>0</v>
+      </c>
+      <c r="S40">
+        <v>-1</v>
+      </c>
+      <c r="T40" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>134</v>
+      </c>
+      <c r="B41" t="s">
+        <v>107</v>
+      </c>
+      <c r="C41" t="s">
+        <v>112</v>
+      </c>
+      <c r="D41" t="s">
+        <v>60</v>
+      </c>
+      <c r="F41" t="b">
+        <v>0</v>
+      </c>
+      <c r="G41" t="b">
+        <v>1</v>
+      </c>
+      <c r="H41" t="b">
+        <v>1</v>
+      </c>
+      <c r="I41" t="b">
+        <v>1</v>
+      </c>
+      <c r="L41" t="s">
+        <v>29</v>
+      </c>
+      <c r="M41" t="b">
+        <v>0</v>
+      </c>
+      <c r="N41">
+        <v>-1</v>
+      </c>
+      <c r="Q41" t="s">
+        <v>29</v>
+      </c>
+      <c r="R41" t="b">
+        <v>0</v>
+      </c>
+      <c r="S41">
+        <v>-1</v>
+      </c>
+      <c r="T41" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>134</v>
+      </c>
+      <c r="B42" t="s">
+        <v>110</v>
+      </c>
+      <c r="C42" t="s">
+        <v>147</v>
+      </c>
+      <c r="D42" t="s">
+        <v>1</v>
+      </c>
+      <c r="F42" t="b">
+        <v>0</v>
+      </c>
+      <c r="G42" t="b">
+        <v>0</v>
+      </c>
+      <c r="H42" t="b">
+        <v>1</v>
+      </c>
+      <c r="I42" t="b">
+        <v>1</v>
+      </c>
+      <c r="L42" t="s">
+        <v>29</v>
+      </c>
+      <c r="M42" t="b">
+        <v>0</v>
+      </c>
+      <c r="N42">
+        <v>200</v>
+      </c>
+      <c r="O42" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q42" t="s">
+        <v>29</v>
+      </c>
+      <c r="R42" t="b">
+        <v>0</v>
+      </c>
+      <c r="S42">
+        <v>-1</v>
+      </c>
+      <c r="T42">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>134</v>
+      </c>
+      <c r="B43" t="s">
+        <v>108</v>
+      </c>
+      <c r="C43" t="s">
+        <v>113</v>
+      </c>
+      <c r="D43" t="s">
+        <v>1</v>
+      </c>
+      <c r="F43" t="b">
+        <v>0</v>
+      </c>
+      <c r="G43" t="b">
+        <v>0</v>
+      </c>
+      <c r="H43" t="b">
+        <v>1</v>
+      </c>
+      <c r="I43" t="b">
+        <v>1</v>
+      </c>
+      <c r="L43" t="s">
+        <v>29</v>
+      </c>
+      <c r="M43" t="b">
+        <v>0</v>
+      </c>
+      <c r="N43">
+        <v>200</v>
+      </c>
+      <c r="O43" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q43" t="s">
+        <v>29</v>
+      </c>
+      <c r="R43" t="b">
+        <v>0</v>
+      </c>
+      <c r="S43">
+        <v>-1</v>
+      </c>
+      <c r="T43">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>134</v>
+      </c>
+      <c r="B44" t="s">
+        <v>111</v>
+      </c>
+      <c r="C44" t="s">
+        <v>148</v>
+      </c>
+      <c r="D44" t="s">
+        <v>1</v>
+      </c>
+      <c r="F44" t="b">
+        <v>0</v>
+      </c>
+      <c r="G44" t="b">
+        <v>0</v>
+      </c>
+      <c r="H44" t="b">
+        <v>1</v>
+      </c>
+      <c r="I44" t="b">
+        <v>1</v>
+      </c>
+      <c r="L44" t="s">
+        <v>29</v>
+      </c>
+      <c r="M44" t="b">
+        <v>0</v>
+      </c>
+      <c r="N44">
+        <v>150</v>
+      </c>
+      <c r="O44" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q44" t="s">
+        <v>29</v>
+      </c>
+      <c r="R44" t="b">
+        <v>0</v>
+      </c>
+      <c r="S44">
+        <v>-1</v>
+      </c>
+      <c r="T44">
+        <v>-1</v>
       </c>
     </row>
   </sheetData>
@@ -3392,10 +3985,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3575,6 +4168,125 @@
       </c>
       <c r="E10" t="s">
         <v>122</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>146</v>
+      </c>
+      <c r="B11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>756150000</v>
+      </c>
+      <c r="E11" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>146</v>
+      </c>
+      <c r="B12" t="s">
+        <v>146</v>
+      </c>
+      <c r="C12" t="b">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>100000000</v>
+      </c>
+      <c r="E12" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>146</v>
+      </c>
+      <c r="B13" t="s">
+        <v>146</v>
+      </c>
+      <c r="C13" t="b">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>100000005</v>
+      </c>
+      <c r="E13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>146</v>
+      </c>
+      <c r="B14" t="s">
+        <v>146</v>
+      </c>
+      <c r="C14" t="b">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>100000003</v>
+      </c>
+      <c r="E14" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>146</v>
+      </c>
+      <c r="B15" t="s">
+        <v>146</v>
+      </c>
+      <c r="C15" t="b">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>100000001</v>
+      </c>
+      <c r="E15" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>146</v>
+      </c>
+      <c r="B16" t="s">
+        <v>146</v>
+      </c>
+      <c r="C16" t="b">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>100000004</v>
+      </c>
+      <c r="E16" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>146</v>
+      </c>
+      <c r="B17" t="s">
+        <v>146</v>
+      </c>
+      <c r="C17" t="b">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>100000002</v>
+      </c>
+      <c r="E17" t="s">
+        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added type configuration for portal web links + implemented import where config only unique fields
</commit_message>
<xml_diff>
--- a/SolutionItems/Customisations.xlsx
+++ b/SolutionItems/Customisations.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="23820" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="23820" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Record Types" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="167">
   <si>
     <t>Relationship Name</t>
   </si>
@@ -469,6 +469,60 @@
   </si>
   <si>
     <t>Subgrid Name</t>
+  </si>
+  <si>
+    <t>Web Link</t>
+  </si>
+  <si>
+    <t>adx_weblink</t>
+  </si>
+  <si>
+    <t>Web Links</t>
+  </si>
+  <si>
+    <t>A textual or imaged based link to an interal or external URL.</t>
+  </si>
+  <si>
+    <t>Web Link Set</t>
+  </si>
+  <si>
+    <t>adx_weblinkset</t>
+  </si>
+  <si>
+    <t>Web Link Sets</t>
+  </si>
+  <si>
+    <t>A grouping of web links.</t>
+  </si>
+  <si>
+    <t>adx_parentweblinkid</t>
+  </si>
+  <si>
+    <t>Parent Web Link</t>
+  </si>
+  <si>
+    <t>Unique identifier for parent Web Link associated with Web Link.</t>
+  </si>
+  <si>
+    <t>adx_weblinksetid</t>
+  </si>
+  <si>
+    <t>Unique identifier for Web Link Set associated with Web Link.</t>
+  </si>
+  <si>
+    <t>Shows the name of the custom entity.</t>
+  </si>
+  <si>
+    <t>Website</t>
+  </si>
+  <si>
+    <t>adx_website</t>
+  </si>
+  <si>
+    <t>Websites</t>
+  </si>
+  <si>
+    <t>Web Portal</t>
   </si>
 </sst>
 </file>
@@ -828,10 +882,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K14"/>
+  <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+      <selection activeCell="L1" sqref="L1:R1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1333,6 +1387,111 @@
         <v>0</v>
       </c>
     </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>149</v>
+      </c>
+      <c r="B15" t="s">
+        <v>150</v>
+      </c>
+      <c r="C15" t="s">
+        <v>151</v>
+      </c>
+      <c r="D15" t="s">
+        <v>152</v>
+      </c>
+      <c r="E15" t="b">
+        <v>0</v>
+      </c>
+      <c r="F15" t="b">
+        <v>0</v>
+      </c>
+      <c r="G15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H15" t="b">
+        <v>0</v>
+      </c>
+      <c r="I15" t="b">
+        <v>0</v>
+      </c>
+      <c r="J15" t="b">
+        <v>1</v>
+      </c>
+      <c r="K15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>153</v>
+      </c>
+      <c r="B16" t="s">
+        <v>154</v>
+      </c>
+      <c r="C16" t="s">
+        <v>155</v>
+      </c>
+      <c r="D16" t="s">
+        <v>156</v>
+      </c>
+      <c r="E16" t="b">
+        <v>0</v>
+      </c>
+      <c r="F16" t="b">
+        <v>0</v>
+      </c>
+      <c r="G16" t="b">
+        <v>0</v>
+      </c>
+      <c r="H16" t="b">
+        <v>0</v>
+      </c>
+      <c r="I16" t="b">
+        <v>0</v>
+      </c>
+      <c r="J16" t="b">
+        <v>1</v>
+      </c>
+      <c r="K16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>163</v>
+      </c>
+      <c r="B17" t="s">
+        <v>164</v>
+      </c>
+      <c r="C17" t="s">
+        <v>165</v>
+      </c>
+      <c r="D17" t="s">
+        <v>166</v>
+      </c>
+      <c r="E17" t="b">
+        <v>0</v>
+      </c>
+      <c r="F17" t="b">
+        <v>0</v>
+      </c>
+      <c r="G17" t="b">
+        <v>1</v>
+      </c>
+      <c r="H17" t="b">
+        <v>1</v>
+      </c>
+      <c r="I17" t="b">
+        <v>1</v>
+      </c>
+      <c r="J17" t="b">
+        <v>1</v>
+      </c>
+      <c r="K17" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1341,10 +1500,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T44"/>
+  <dimension ref="A1:T49"/>
   <sheetViews>
-    <sheetView topLeftCell="N7" workbookViewId="0">
-      <selection activeCell="T33" sqref="T33"/>
+    <sheetView tabSelected="1" topLeftCell="M13" workbookViewId="0">
+      <selection activeCell="AA21" sqref="AA21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3960,6 +4119,265 @@
         <v>-1</v>
       </c>
       <c r="T44">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>150</v>
+      </c>
+      <c r="B45" t="s">
+        <v>93</v>
+      </c>
+      <c r="C45" t="s">
+        <v>12</v>
+      </c>
+      <c r="D45" t="s">
+        <v>1</v>
+      </c>
+      <c r="E45" t="s">
+        <v>162</v>
+      </c>
+      <c r="F45" t="b">
+        <v>1</v>
+      </c>
+      <c r="G45" t="b">
+        <v>1</v>
+      </c>
+      <c r="H45" t="b">
+        <v>1</v>
+      </c>
+      <c r="I45" t="b">
+        <v>1</v>
+      </c>
+      <c r="L45" t="s">
+        <v>29</v>
+      </c>
+      <c r="M45" t="b">
+        <v>0</v>
+      </c>
+      <c r="N45">
+        <v>100</v>
+      </c>
+      <c r="O45" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q45" t="s">
+        <v>29</v>
+      </c>
+      <c r="R45" t="b">
+        <v>0</v>
+      </c>
+      <c r="S45">
+        <v>-1</v>
+      </c>
+      <c r="T45">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>150</v>
+      </c>
+      <c r="B46" t="s">
+        <v>157</v>
+      </c>
+      <c r="C46" t="s">
+        <v>158</v>
+      </c>
+      <c r="D46" t="s">
+        <v>59</v>
+      </c>
+      <c r="E46" t="s">
+        <v>159</v>
+      </c>
+      <c r="F46" t="b">
+        <v>0</v>
+      </c>
+      <c r="G46" t="b">
+        <v>0</v>
+      </c>
+      <c r="H46" t="b">
+        <v>0</v>
+      </c>
+      <c r="I46" t="b">
+        <v>1</v>
+      </c>
+      <c r="L46" t="s">
+        <v>150</v>
+      </c>
+      <c r="M46" t="b">
+        <v>1</v>
+      </c>
+      <c r="N46">
+        <v>-1</v>
+      </c>
+      <c r="Q46" t="s">
+        <v>29</v>
+      </c>
+      <c r="R46" t="b">
+        <v>0</v>
+      </c>
+      <c r="S46">
+        <v>-1</v>
+      </c>
+      <c r="T46">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>150</v>
+      </c>
+      <c r="B47" t="s">
+        <v>160</v>
+      </c>
+      <c r="C47" t="s">
+        <v>153</v>
+      </c>
+      <c r="D47" t="s">
+        <v>59</v>
+      </c>
+      <c r="E47" t="s">
+        <v>161</v>
+      </c>
+      <c r="F47" t="b">
+        <v>0</v>
+      </c>
+      <c r="G47" t="b">
+        <v>1</v>
+      </c>
+      <c r="H47" t="b">
+        <v>0</v>
+      </c>
+      <c r="I47" t="b">
+        <v>1</v>
+      </c>
+      <c r="L47" t="s">
+        <v>154</v>
+      </c>
+      <c r="M47" t="b">
+        <v>1</v>
+      </c>
+      <c r="N47">
+        <v>-1</v>
+      </c>
+      <c r="Q47" t="s">
+        <v>29</v>
+      </c>
+      <c r="R47" t="b">
+        <v>0</v>
+      </c>
+      <c r="S47">
+        <v>-1</v>
+      </c>
+      <c r="T47">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>154</v>
+      </c>
+      <c r="B48" t="s">
+        <v>93</v>
+      </c>
+      <c r="C48" t="s">
+        <v>12</v>
+      </c>
+      <c r="D48" t="s">
+        <v>1</v>
+      </c>
+      <c r="E48" t="s">
+        <v>162</v>
+      </c>
+      <c r="F48" t="b">
+        <v>1</v>
+      </c>
+      <c r="G48" t="b">
+        <v>1</v>
+      </c>
+      <c r="H48" t="b">
+        <v>1</v>
+      </c>
+      <c r="I48" t="b">
+        <v>1</v>
+      </c>
+      <c r="L48" t="s">
+        <v>29</v>
+      </c>
+      <c r="M48" t="b">
+        <v>0</v>
+      </c>
+      <c r="N48">
+        <v>100</v>
+      </c>
+      <c r="O48" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q48" t="s">
+        <v>29</v>
+      </c>
+      <c r="R48" t="b">
+        <v>0</v>
+      </c>
+      <c r="S48">
+        <v>-1</v>
+      </c>
+      <c r="T48">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>164</v>
+      </c>
+      <c r="B49" t="s">
+        <v>93</v>
+      </c>
+      <c r="C49" t="s">
+        <v>12</v>
+      </c>
+      <c r="D49" t="s">
+        <v>1</v>
+      </c>
+      <c r="E49" t="s">
+        <v>162</v>
+      </c>
+      <c r="F49" t="b">
+        <v>1</v>
+      </c>
+      <c r="G49" t="b">
+        <v>1</v>
+      </c>
+      <c r="H49" t="b">
+        <v>1</v>
+      </c>
+      <c r="I49" t="b">
+        <v>1</v>
+      </c>
+      <c r="L49" t="s">
+        <v>29</v>
+      </c>
+      <c r="M49" t="b">
+        <v>0</v>
+      </c>
+      <c r="N49">
+        <v>100</v>
+      </c>
+      <c r="O49" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q49" t="s">
+        <v>29</v>
+      </c>
+      <c r="R49" t="b">
+        <v>0</v>
+      </c>
+      <c r="S49">
+        <v>-1</v>
+      </c>
+      <c r="T49">
         <v>-1</v>
       </c>
     </row>
@@ -3987,8 +4405,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Add VSIX feature to export portal code into visual studio sproject + fix scripts deleting fake setting files
</commit_message>
<xml_diff>
--- a/SolutionItems/Customisations.xlsx
+++ b/SolutionItems/Customisations.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="23820" windowHeight="8010" activeTab="1"/>
+    <workbookView minimized="1" xWindow="120" yWindow="120" windowWidth="23820" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Record Types" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="670" uniqueCount="182">
   <si>
     <t>Relationship Name</t>
   </si>
@@ -523,6 +523,51 @@
   </si>
   <si>
     <t>Web Portal</t>
+  </si>
+  <si>
+    <t>adx_websiteid</t>
+  </si>
+  <si>
+    <t>adx_webtemplate</t>
+  </si>
+  <si>
+    <t>Web Template</t>
+  </si>
+  <si>
+    <t>Web Templates</t>
+  </si>
+  <si>
+    <t>Entity List</t>
+  </si>
+  <si>
+    <t>adx_entitylist</t>
+  </si>
+  <si>
+    <t>Entity Lists</t>
+  </si>
+  <si>
+    <t>adx_copy</t>
+  </si>
+  <si>
+    <t>Copy</t>
+  </si>
+  <si>
+    <t>adx_customjavascript</t>
+  </si>
+  <si>
+    <t>Custom JavaScript</t>
+  </si>
+  <si>
+    <t>adx_customcss</t>
+  </si>
+  <si>
+    <t>Custom CSS</t>
+  </si>
+  <si>
+    <t>adx_source</t>
+  </si>
+  <si>
+    <t>adx_registerstartupscript</t>
   </si>
 </sst>
 </file>
@@ -882,10 +927,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K17"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:R1048576"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1492,6 +1537,76 @@
         <v>0</v>
       </c>
     </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>169</v>
+      </c>
+      <c r="B18" t="s">
+        <v>168</v>
+      </c>
+      <c r="C18" t="s">
+        <v>170</v>
+      </c>
+      <c r="D18" t="s">
+        <v>170</v>
+      </c>
+      <c r="E18" t="b">
+        <v>0</v>
+      </c>
+      <c r="F18" t="b">
+        <v>0</v>
+      </c>
+      <c r="G18" t="b">
+        <v>1</v>
+      </c>
+      <c r="H18" t="b">
+        <v>1</v>
+      </c>
+      <c r="I18" t="b">
+        <v>1</v>
+      </c>
+      <c r="J18" t="b">
+        <v>1</v>
+      </c>
+      <c r="K18" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>171</v>
+      </c>
+      <c r="B19" t="s">
+        <v>172</v>
+      </c>
+      <c r="C19" t="s">
+        <v>173</v>
+      </c>
+      <c r="D19" t="s">
+        <v>173</v>
+      </c>
+      <c r="E19" t="b">
+        <v>0</v>
+      </c>
+      <c r="F19" t="b">
+        <v>0</v>
+      </c>
+      <c r="G19" t="b">
+        <v>1</v>
+      </c>
+      <c r="H19" t="b">
+        <v>1</v>
+      </c>
+      <c r="I19" t="b">
+        <v>1</v>
+      </c>
+      <c r="J19" t="b">
+        <v>1</v>
+      </c>
+      <c r="K19" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1500,16 +1615,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T49"/>
+  <dimension ref="A1:T64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M13" workbookViewId="0">
-      <selection activeCell="AA21" sqref="AA21"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" customWidth="1"/>
+    <col min="2" max="2" width="25.5703125" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
     <col min="4" max="4" width="15.5703125" customWidth="1"/>
     <col min="5" max="6" width="24" customWidth="1"/>
@@ -2760,67 +2875,71 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:20" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F21" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G21" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="H21" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="I21" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="J21" s="2">
-        <v>1</v>
-      </c>
-      <c r="K21" s="2">
-        <v>200</v>
-      </c>
-      <c r="L21" s="2"/>
-      <c r="M21" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="N21" s="2">
-        <v>200</v>
-      </c>
-      <c r="O21" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B21" t="s">
+        <v>167</v>
+      </c>
+      <c r="C21" t="s">
+        <v>163</v>
+      </c>
+      <c r="D21" t="s">
+        <v>59</v>
+      </c>
+      <c r="E21" t="s">
+        <v>163</v>
+      </c>
+      <c r="F21" t="b">
+        <v>0</v>
+      </c>
+      <c r="G21" t="b">
+        <v>0</v>
+      </c>
+      <c r="H21" t="b">
+        <v>0</v>
+      </c>
+      <c r="I21" t="b">
+        <v>1</v>
+      </c>
+      <c r="J21">
+        <v>1</v>
+      </c>
+      <c r="K21">
+        <v>200</v>
+      </c>
+      <c r="L21" t="s">
+        <v>164</v>
+      </c>
+      <c r="M21" t="b">
+        <v>1</v>
+      </c>
+      <c r="N21">
+        <v>202</v>
+      </c>
+      <c r="O21" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="P21" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q21" s="4">
-        <v>0</v>
-      </c>
-      <c r="R21" s="4">
-        <v>0</v>
-      </c>
-      <c r="S21" s="4"/>
+      <c r="P21" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q21" s="1">
+        <v>-100000000</v>
+      </c>
+      <c r="R21" s="1">
+        <v>100000000</v>
+      </c>
+      <c r="S21" s="1">
+        <v>0</v>
+      </c>
       <c r="T21" s="1" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="22" spans="1:20" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>93</v>
@@ -2878,7 +2997,7 @@
     </row>
     <row r="23" spans="1:20" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>93</v>
@@ -2936,7 +3055,7 @@
     </row>
     <row r="24" spans="1:20" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>93</v>
@@ -2992,64 +3111,60 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="B25" t="s">
-        <v>98</v>
-      </c>
-      <c r="C25" t="s">
-        <v>99</v>
-      </c>
-      <c r="D25" t="s">
-        <v>59</v>
-      </c>
-      <c r="E25" t="s">
-        <v>99</v>
-      </c>
-      <c r="F25" t="b">
-        <v>0</v>
-      </c>
-      <c r="G25" t="b">
-        <v>0</v>
-      </c>
-      <c r="H25" t="b">
-        <v>0</v>
-      </c>
-      <c r="I25" t="b">
-        <v>1</v>
-      </c>
-      <c r="J25">
-        <v>1</v>
-      </c>
-      <c r="K25">
-        <v>200</v>
-      </c>
-      <c r="L25" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="M25" t="b">
-        <v>1</v>
-      </c>
-      <c r="N25">
-        <v>202</v>
-      </c>
-      <c r="O25" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F25" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G25" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H25" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I25" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="J25" s="2">
+        <v>1</v>
+      </c>
+      <c r="K25" s="2">
+        <v>200</v>
+      </c>
+      <c r="L25" s="2"/>
+      <c r="M25" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="N25" s="2">
+        <v>200</v>
+      </c>
+      <c r="O25" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="P25" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q25" s="1">
-        <v>-100000000</v>
-      </c>
-      <c r="R25" s="1">
-        <v>100000000</v>
-      </c>
-      <c r="S25" s="1">
-        <v>0</v>
-      </c>
+      <c r="P25" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q25" s="4">
+        <v>0</v>
+      </c>
+      <c r="R25" s="4">
+        <v>0</v>
+      </c>
+      <c r="S25" s="4"/>
       <c r="T25" s="1" t="s">
         <v>29</v>
       </c>
@@ -3059,16 +3174,16 @@
         <v>94</v>
       </c>
       <c r="B26" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="C26" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="D26" t="s">
         <v>59</v>
       </c>
       <c r="E26" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="F26" t="b">
         <v>0</v>
@@ -3089,7 +3204,7 @@
         <v>200</v>
       </c>
       <c r="L26" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="M26" t="b">
         <v>1</v>
@@ -3118,19 +3233,19 @@
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B27" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C27" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D27" t="s">
         <v>59</v>
       </c>
       <c r="E27" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="F27" t="b">
         <v>0</v>
@@ -3151,7 +3266,7 @@
         <v>200</v>
       </c>
       <c r="L27" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="M27" t="b">
         <v>1</v>
@@ -3178,137 +3293,145 @@
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:20" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F28" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G28" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="H28" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="I28" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="J28" s="2">
-        <v>1</v>
-      </c>
-      <c r="K28" s="2">
-        <v>200</v>
-      </c>
-      <c r="L28" s="2"/>
-      <c r="M28" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="N28" s="2">
-        <v>200</v>
-      </c>
-      <c r="O28" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B28" t="s">
+        <v>167</v>
+      </c>
+      <c r="C28" t="s">
+        <v>163</v>
+      </c>
+      <c r="D28" t="s">
+        <v>59</v>
+      </c>
+      <c r="E28" t="s">
+        <v>163</v>
+      </c>
+      <c r="F28" t="b">
+        <v>0</v>
+      </c>
+      <c r="G28" t="b">
+        <v>0</v>
+      </c>
+      <c r="H28" t="b">
+        <v>0</v>
+      </c>
+      <c r="I28" t="b">
+        <v>1</v>
+      </c>
+      <c r="J28">
+        <v>1</v>
+      </c>
+      <c r="K28">
+        <v>200</v>
+      </c>
+      <c r="L28" t="s">
+        <v>164</v>
+      </c>
+      <c r="M28" t="b">
+        <v>1</v>
+      </c>
+      <c r="N28">
+        <v>202</v>
+      </c>
+      <c r="O28" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="P28" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q28" s="4">
-        <v>0</v>
-      </c>
-      <c r="R28" s="4">
-        <v>0</v>
-      </c>
-      <c r="S28" s="4"/>
+      <c r="P28" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q28" s="1">
+        <v>-100000000</v>
+      </c>
+      <c r="R28" s="1">
+        <v>100000000</v>
+      </c>
+      <c r="S28" s="1">
+        <v>0</v>
+      </c>
       <c r="T28" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="29" spans="1:20" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F29" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G29" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="H29" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="I29" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="J29" s="2">
-        <v>1</v>
-      </c>
-      <c r="K29" s="2">
-        <v>200</v>
-      </c>
-      <c r="L29" s="2"/>
-      <c r="M29" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="N29" s="2">
-        <v>200</v>
-      </c>
-      <c r="O29" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B29" t="s">
+        <v>174</v>
+      </c>
+      <c r="C29" t="s">
+        <v>175</v>
+      </c>
+      <c r="D29" t="s">
+        <v>69</v>
+      </c>
+      <c r="E29" t="s">
+        <v>175</v>
+      </c>
+      <c r="F29" t="b">
+        <v>0</v>
+      </c>
+      <c r="G29" t="b">
+        <v>0</v>
+      </c>
+      <c r="H29" t="b">
+        <v>0</v>
+      </c>
+      <c r="I29" t="b">
+        <v>1</v>
+      </c>
+      <c r="J29">
+        <v>1</v>
+      </c>
+      <c r="K29">
+        <v>200</v>
+      </c>
+      <c r="L29" t="s">
+        <v>29</v>
+      </c>
+      <c r="M29" t="b">
+        <v>0</v>
+      </c>
+      <c r="N29">
+        <v>4000</v>
+      </c>
+      <c r="O29" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="P29" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q29" s="4">
-        <v>0</v>
-      </c>
-      <c r="R29" s="4">
-        <v>0</v>
-      </c>
-      <c r="S29" s="4"/>
+      <c r="P29" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q29" s="1">
+        <v>0</v>
+      </c>
+      <c r="R29" s="1">
+        <v>0</v>
+      </c>
+      <c r="S29" s="1">
+        <v>0</v>
+      </c>
       <c r="T29" s="1" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="B30" t="s">
-        <v>105</v>
+        <v>176</v>
       </c>
       <c r="C30" t="s">
-        <v>123</v>
+        <v>177</v>
       </c>
       <c r="D30" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="E30" t="s">
-        <v>123</v>
+        <v>177</v>
       </c>
       <c r="F30" t="b">
         <v>0</v>
@@ -3328,14 +3451,14 @@
       <c r="K30">
         <v>200</v>
       </c>
-      <c r="L30" s="2" t="s">
-        <v>105</v>
+      <c r="L30" t="s">
+        <v>29</v>
       </c>
       <c r="M30" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N30">
-        <v>202</v>
+        <v>4000</v>
       </c>
       <c r="O30" s="1" t="s">
         <v>30</v>
@@ -3344,10 +3467,10 @@
         <v>0</v>
       </c>
       <c r="Q30" s="1">
-        <v>-100000000</v>
+        <v>0</v>
       </c>
       <c r="R30" s="1">
-        <v>100000000</v>
+        <v>0</v>
       </c>
       <c r="S30" s="1">
         <v>0</v>
@@ -3358,19 +3481,19 @@
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="B31" t="s">
-        <v>107</v>
+        <v>178</v>
       </c>
       <c r="C31" t="s">
-        <v>112</v>
+        <v>179</v>
       </c>
       <c r="D31" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="E31" t="s">
-        <v>112</v>
+        <v>179</v>
       </c>
       <c r="F31" t="b">
         <v>0</v>
@@ -3391,13 +3514,13 @@
         <v>200</v>
       </c>
       <c r="L31" t="s">
-        <v>56</v>
+        <v>29</v>
       </c>
       <c r="M31" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N31">
-        <v>203</v>
+        <v>4000</v>
       </c>
       <c r="O31" s="1" t="s">
         <v>30</v>
@@ -3406,33 +3529,33 @@
         <v>0</v>
       </c>
       <c r="Q31" s="1">
-        <v>-100000000</v>
+        <v>0</v>
       </c>
       <c r="R31" s="1">
-        <v>100000000</v>
+        <v>0</v>
       </c>
       <c r="S31" s="1">
         <v>0</v>
       </c>
-      <c r="T31" t="s">
-        <v>117</v>
+      <c r="T31" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="B32" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="C32" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="D32" t="s">
-        <v>1</v>
+        <v>59</v>
       </c>
       <c r="E32" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="F32" t="b">
         <v>0</v>
@@ -3452,14 +3575,14 @@
       <c r="K32">
         <v>200</v>
       </c>
-      <c r="L32" t="s">
-        <v>29</v>
+      <c r="L32" s="2" t="s">
+        <v>94</v>
       </c>
       <c r="M32" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N32">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="O32" s="1" t="s">
         <v>30</v>
@@ -3468,10 +3591,10 @@
         <v>0</v>
       </c>
       <c r="Q32" s="1">
-        <v>0</v>
+        <v>-100000000</v>
       </c>
       <c r="R32" s="1">
-        <v>0</v>
+        <v>100000000</v>
       </c>
       <c r="S32" s="1">
         <v>0</v>
@@ -3480,83 +3603,79 @@
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:20" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="B33" t="s">
-        <v>109</v>
-      </c>
-      <c r="C33" t="s">
-        <v>114</v>
-      </c>
-      <c r="D33" t="s">
-        <v>1</v>
-      </c>
-      <c r="E33" t="s">
-        <v>114</v>
-      </c>
-      <c r="F33" t="b">
-        <v>0</v>
-      </c>
-      <c r="G33" t="b">
-        <v>0</v>
-      </c>
-      <c r="H33" t="b">
-        <v>0</v>
-      </c>
-      <c r="I33" t="b">
-        <v>1</v>
-      </c>
-      <c r="J33">
-        <v>1</v>
-      </c>
-      <c r="K33">
-        <v>200</v>
-      </c>
-      <c r="L33" t="s">
-        <v>29</v>
-      </c>
-      <c r="M33" t="b">
-        <v>0</v>
-      </c>
-      <c r="N33">
-        <v>201</v>
-      </c>
-      <c r="O33" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F33" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G33" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H33" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I33" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="J33" s="2">
+        <v>1</v>
+      </c>
+      <c r="K33" s="2">
+        <v>200</v>
+      </c>
+      <c r="L33" s="2"/>
+      <c r="M33" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="N33" s="2">
+        <v>200</v>
+      </c>
+      <c r="O33" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="P33" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q33" s="1">
-        <v>0</v>
-      </c>
-      <c r="R33" s="1">
-        <v>0</v>
-      </c>
-      <c r="S33" s="1">
-        <v>0</v>
-      </c>
+      <c r="P33" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q33" s="4">
+        <v>0</v>
+      </c>
+      <c r="R33" s="4">
+        <v>0</v>
+      </c>
+      <c r="S33" s="4"/>
       <c r="T33" s="1" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B34" t="s">
-        <v>110</v>
+        <v>167</v>
       </c>
       <c r="C34" t="s">
-        <v>115</v>
+        <v>163</v>
       </c>
       <c r="D34" t="s">
-        <v>1</v>
+        <v>59</v>
       </c>
       <c r="E34" t="s">
-        <v>115</v>
+        <v>163</v>
       </c>
       <c r="F34" t="b">
         <v>0</v>
@@ -3577,10 +3696,10 @@
         <v>200</v>
       </c>
       <c r="L34" t="s">
-        <v>29</v>
+        <v>164</v>
       </c>
       <c r="M34" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N34">
         <v>202</v>
@@ -3592,10 +3711,10 @@
         <v>0</v>
       </c>
       <c r="Q34" s="1">
-        <v>0</v>
+        <v>-100000000</v>
       </c>
       <c r="R34" s="1">
-        <v>0</v>
+        <v>100000000</v>
       </c>
       <c r="S34" s="1">
         <v>0</v>
@@ -3606,19 +3725,19 @@
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B35" t="s">
-        <v>111</v>
+        <v>181</v>
       </c>
       <c r="C35" t="s">
-        <v>116</v>
+        <v>177</v>
       </c>
       <c r="D35" t="s">
-        <v>1</v>
+        <v>69</v>
       </c>
       <c r="E35" t="s">
-        <v>116</v>
+        <v>177</v>
       </c>
       <c r="F35" t="b">
         <v>0</v>
@@ -3645,7 +3764,7 @@
         <v>0</v>
       </c>
       <c r="N35">
-        <v>203</v>
+        <v>4000</v>
       </c>
       <c r="O35" s="1" t="s">
         <v>30</v>
@@ -3666,133 +3785,147 @@
         <v>29</v>
       </c>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>130</v>
-      </c>
-      <c r="B36" t="s">
+    <row r="36" spans="1:20" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B36" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C36" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D36" t="s">
-        <v>1</v>
-      </c>
-      <c r="E36" t="s">
-        <v>140</v>
-      </c>
-      <c r="F36" t="b">
-        <v>1</v>
-      </c>
-      <c r="G36" t="b">
-        <v>1</v>
-      </c>
-      <c r="H36" t="b">
-        <v>1</v>
-      </c>
-      <c r="I36" t="b">
-        <v>1</v>
-      </c>
-      <c r="L36" t="s">
-        <v>29</v>
-      </c>
-      <c r="M36" t="b">
-        <v>0</v>
-      </c>
-      <c r="N36">
-        <v>100</v>
-      </c>
-      <c r="O36" t="s">
+      <c r="D36" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F36" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G36" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H36" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I36" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="J36" s="2">
+        <v>1</v>
+      </c>
+      <c r="K36" s="2">
+        <v>200</v>
+      </c>
+      <c r="L36" s="2"/>
+      <c r="M36" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="N36" s="2">
+        <v>200</v>
+      </c>
+      <c r="O36" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="Q36" t="s">
-        <v>29</v>
-      </c>
-      <c r="R36" t="b">
-        <v>0</v>
-      </c>
-      <c r="S36">
-        <v>-1</v>
-      </c>
+      <c r="P36" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q36" s="4">
+        <v>0</v>
+      </c>
+      <c r="R36" s="4">
+        <v>0</v>
+      </c>
+      <c r="S36" s="4"/>
       <c r="T36" s="1" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>137</v>
+      <c r="A37" s="2" t="s">
+        <v>106</v>
       </c>
       <c r="B37" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
       <c r="C37" t="s">
-        <v>12</v>
+        <v>123</v>
       </c>
       <c r="D37" t="s">
-        <v>1</v>
+        <v>59</v>
       </c>
       <c r="E37" t="s">
-        <v>140</v>
+        <v>123</v>
       </c>
       <c r="F37" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G37" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H37" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I37" t="b">
         <v>1</v>
       </c>
-      <c r="L37" t="s">
-        <v>29</v>
+      <c r="J37">
+        <v>1</v>
+      </c>
+      <c r="K37">
+        <v>200</v>
+      </c>
+      <c r="L37" s="2" t="s">
+        <v>105</v>
       </c>
       <c r="M37" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N37">
-        <v>100</v>
-      </c>
-      <c r="O37" t="s">
+        <v>202</v>
+      </c>
+      <c r="O37" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="Q37" t="s">
-        <v>29</v>
-      </c>
-      <c r="R37" t="b">
-        <v>0</v>
-      </c>
-      <c r="S37">
-        <v>-1</v>
+      <c r="P37" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q37" s="1">
+        <v>-100000000</v>
+      </c>
+      <c r="R37" s="1">
+        <v>100000000</v>
+      </c>
+      <c r="S37" s="1">
+        <v>0</v>
       </c>
       <c r="T37" s="1" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>137</v>
+      <c r="A38" s="2" t="s">
+        <v>106</v>
       </c>
       <c r="B38" t="s">
-        <v>130</v>
+        <v>107</v>
       </c>
       <c r="C38" t="s">
-        <v>129</v>
+        <v>112</v>
       </c>
       <c r="D38" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E38" t="s">
-        <v>141</v>
+        <v>112</v>
       </c>
       <c r="F38" t="b">
         <v>0</v>
       </c>
       <c r="G38" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H38" t="b">
         <v>0</v>
@@ -3800,156 +3933,198 @@
       <c r="I38" t="b">
         <v>1</v>
       </c>
+      <c r="J38">
+        <v>1</v>
+      </c>
+      <c r="K38">
+        <v>200</v>
+      </c>
       <c r="L38" t="s">
-        <v>130</v>
+        <v>56</v>
       </c>
       <c r="M38" t="b">
         <v>1</v>
       </c>
       <c r="N38">
-        <v>-1</v>
-      </c>
-      <c r="Q38" t="s">
-        <v>29</v>
-      </c>
-      <c r="R38" t="b">
-        <v>0</v>
-      </c>
-      <c r="S38">
-        <v>-1</v>
-      </c>
-      <c r="T38" s="1" t="s">
-        <v>29</v>
+        <v>203</v>
+      </c>
+      <c r="O38" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="P38" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q38" s="1">
+        <v>-100000000</v>
+      </c>
+      <c r="R38" s="1">
+        <v>100000000</v>
+      </c>
+      <c r="S38" s="1">
+        <v>0</v>
+      </c>
+      <c r="T38" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>134</v>
+      <c r="A39" s="2" t="s">
+        <v>106</v>
       </c>
       <c r="B39" t="s">
+        <v>108</v>
+      </c>
+      <c r="C39" t="s">
+        <v>113</v>
+      </c>
+      <c r="D39" t="s">
+        <v>1</v>
+      </c>
+      <c r="E39" t="s">
+        <v>113</v>
+      </c>
+      <c r="F39" t="b">
+        <v>0</v>
+      </c>
+      <c r="G39" t="b">
+        <v>0</v>
+      </c>
+      <c r="H39" t="b">
+        <v>0</v>
+      </c>
+      <c r="I39" t="b">
+        <v>1</v>
+      </c>
+      <c r="J39">
+        <v>1</v>
+      </c>
+      <c r="K39">
+        <v>200</v>
+      </c>
+      <c r="L39" t="s">
+        <v>29</v>
+      </c>
+      <c r="M39" t="b">
+        <v>0</v>
+      </c>
+      <c r="N39">
+        <v>200</v>
+      </c>
+      <c r="O39" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="P39" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q39" s="1">
+        <v>0</v>
+      </c>
+      <c r="R39" s="1">
+        <v>0</v>
+      </c>
+      <c r="S39" s="1">
+        <v>0</v>
+      </c>
+      <c r="T39" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B40" t="s">
         <v>109</v>
       </c>
-      <c r="C39" t="s">
-        <v>142</v>
-      </c>
-      <c r="D39" t="s">
-        <v>1</v>
-      </c>
-      <c r="E39" t="s">
-        <v>143</v>
-      </c>
-      <c r="F39" t="b">
-        <v>1</v>
-      </c>
-      <c r="G39" t="b">
-        <v>0</v>
-      </c>
-      <c r="H39" t="b">
-        <v>1</v>
-      </c>
-      <c r="I39" t="b">
-        <v>1</v>
-      </c>
-      <c r="L39" t="s">
-        <v>29</v>
-      </c>
-      <c r="M39" t="b">
-        <v>0</v>
-      </c>
-      <c r="N39">
-        <v>100</v>
-      </c>
-      <c r="O39" t="s">
+      <c r="C40" t="s">
+        <v>114</v>
+      </c>
+      <c r="D40" t="s">
+        <v>1</v>
+      </c>
+      <c r="E40" t="s">
+        <v>114</v>
+      </c>
+      <c r="F40" t="b">
+        <v>0</v>
+      </c>
+      <c r="G40" t="b">
+        <v>0</v>
+      </c>
+      <c r="H40" t="b">
+        <v>0</v>
+      </c>
+      <c r="I40" t="b">
+        <v>1</v>
+      </c>
+      <c r="J40">
+        <v>1</v>
+      </c>
+      <c r="K40">
+        <v>200</v>
+      </c>
+      <c r="L40" t="s">
+        <v>29</v>
+      </c>
+      <c r="M40" t="b">
+        <v>0</v>
+      </c>
+      <c r="N40">
+        <v>201</v>
+      </c>
+      <c r="O40" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="Q39" t="s">
-        <v>29</v>
-      </c>
-      <c r="R39" t="b">
-        <v>0</v>
-      </c>
-      <c r="S39">
-        <v>-1</v>
-      </c>
-      <c r="T39" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>134</v>
-      </c>
-      <c r="B40" t="s">
-        <v>137</v>
-      </c>
-      <c r="C40" t="s">
-        <v>136</v>
-      </c>
-      <c r="D40" t="s">
-        <v>59</v>
-      </c>
-      <c r="E40" t="s">
-        <v>144</v>
-      </c>
-      <c r="F40" t="b">
-        <v>0</v>
-      </c>
-      <c r="G40" t="b">
-        <v>1</v>
-      </c>
-      <c r="H40" t="b">
-        <v>0</v>
-      </c>
-      <c r="I40" t="b">
-        <v>1</v>
-      </c>
-      <c r="L40" t="s">
-        <v>137</v>
-      </c>
-      <c r="M40" t="b">
-        <v>1</v>
-      </c>
-      <c r="N40">
-        <v>-1</v>
-      </c>
-      <c r="Q40" t="s">
-        <v>29</v>
-      </c>
-      <c r="R40" t="b">
-        <v>0</v>
-      </c>
-      <c r="S40">
-        <v>-1</v>
+      <c r="P40" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q40" s="1">
+        <v>0</v>
+      </c>
+      <c r="R40" s="1">
+        <v>0</v>
+      </c>
+      <c r="S40" s="1">
+        <v>0</v>
       </c>
       <c r="T40" s="1" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="41" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>134</v>
+      <c r="A41" s="2" t="s">
+        <v>106</v>
       </c>
       <c r="B41" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="C41" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="D41" t="s">
-        <v>60</v>
+        <v>1</v>
+      </c>
+      <c r="E41" t="s">
+        <v>115</v>
       </c>
       <c r="F41" t="b">
         <v>0</v>
       </c>
       <c r="G41" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H41" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I41" t="b">
         <v>1</v>
       </c>
+      <c r="J41">
+        <v>1</v>
+      </c>
+      <c r="K41">
+        <v>200</v>
+      </c>
       <c r="L41" t="s">
         <v>29</v>
       </c>
@@ -3957,34 +4132,43 @@
         <v>0</v>
       </c>
       <c r="N41">
-        <v>-1</v>
-      </c>
-      <c r="Q41" t="s">
-        <v>29</v>
-      </c>
-      <c r="R41" t="b">
-        <v>0</v>
-      </c>
-      <c r="S41">
-        <v>-1</v>
-      </c>
-      <c r="T41" t="s">
-        <v>146</v>
+        <v>202</v>
+      </c>
+      <c r="O41" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="P41" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q41" s="1">
+        <v>0</v>
+      </c>
+      <c r="R41" s="1">
+        <v>0</v>
+      </c>
+      <c r="S41" s="1">
+        <v>0</v>
+      </c>
+      <c r="T41" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="42" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>134</v>
+      <c r="A42" s="2" t="s">
+        <v>106</v>
       </c>
       <c r="B42" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C42" t="s">
-        <v>147</v>
+        <v>116</v>
       </c>
       <c r="D42" t="s">
         <v>1</v>
       </c>
+      <c r="E42" t="s">
+        <v>116</v>
+      </c>
       <c r="F42" t="b">
         <v>0</v>
       </c>
@@ -3992,11 +4176,17 @@
         <v>0</v>
       </c>
       <c r="H42" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I42" t="b">
         <v>1</v>
       </c>
+      <c r="J42">
+        <v>1</v>
+      </c>
+      <c r="K42">
+        <v>200</v>
+      </c>
       <c r="L42" t="s">
         <v>29</v>
       </c>
@@ -4004,42 +4194,48 @@
         <v>0</v>
       </c>
       <c r="N42">
-        <v>200</v>
-      </c>
-      <c r="O42" t="s">
+        <v>203</v>
+      </c>
+      <c r="O42" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="Q42" t="s">
-        <v>29</v>
-      </c>
-      <c r="R42" t="b">
-        <v>0</v>
-      </c>
-      <c r="S42">
-        <v>-1</v>
-      </c>
-      <c r="T42">
-        <v>-1</v>
+      <c r="P42" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q42" s="1">
+        <v>0</v>
+      </c>
+      <c r="R42" s="1">
+        <v>0</v>
+      </c>
+      <c r="S42" s="1">
+        <v>0</v>
+      </c>
+      <c r="T42" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B43" t="s">
-        <v>108</v>
+        <v>93</v>
       </c>
       <c r="C43" t="s">
-        <v>113</v>
+        <v>12</v>
       </c>
       <c r="D43" t="s">
         <v>1</v>
       </c>
+      <c r="E43" t="s">
+        <v>140</v>
+      </c>
       <c r="F43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H43" t="b">
         <v>1</v>
@@ -4054,7 +4250,7 @@
         <v>0</v>
       </c>
       <c r="N43">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="O43" t="s">
         <v>30</v>
@@ -4068,22 +4264,25 @@
       <c r="S43">
         <v>-1</v>
       </c>
-      <c r="T43">
-        <v>-1</v>
+      <c r="T43" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B44" t="s">
-        <v>111</v>
+        <v>167</v>
       </c>
       <c r="C44" t="s">
-        <v>148</v>
+        <v>163</v>
       </c>
       <c r="D44" t="s">
-        <v>1</v>
+        <v>59</v>
+      </c>
+      <c r="E44" t="s">
+        <v>163</v>
       </c>
       <c r="F44" t="b">
         <v>0</v>
@@ -4092,39 +4291,48 @@
         <v>0</v>
       </c>
       <c r="H44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I44" t="b">
         <v>1</v>
       </c>
+      <c r="J44">
+        <v>1</v>
+      </c>
+      <c r="K44">
+        <v>200</v>
+      </c>
       <c r="L44" t="s">
-        <v>29</v>
+        <v>164</v>
       </c>
       <c r="M44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N44">
-        <v>150</v>
-      </c>
-      <c r="O44" t="s">
+        <v>202</v>
+      </c>
+      <c r="O44" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="Q44" t="s">
-        <v>29</v>
-      </c>
-      <c r="R44" t="b">
-        <v>0</v>
-      </c>
-      <c r="S44">
-        <v>-1</v>
-      </c>
-      <c r="T44">
-        <v>-1</v>
+      <c r="P44" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q44" s="1">
+        <v>-100000000</v>
+      </c>
+      <c r="R44" s="1">
+        <v>100000000</v>
+      </c>
+      <c r="S44" s="1">
+        <v>0</v>
+      </c>
+      <c r="T44" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="B45" t="s">
         <v>93</v>
@@ -4136,7 +4344,7 @@
         <v>1</v>
       </c>
       <c r="E45" t="s">
-        <v>162</v>
+        <v>140</v>
       </c>
       <c r="F45" t="b">
         <v>1</v>
@@ -4171,31 +4379,31 @@
       <c r="S45">
         <v>-1</v>
       </c>
-      <c r="T45">
-        <v>-1</v>
+      <c r="T45" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="B46" t="s">
-        <v>157</v>
+        <v>130</v>
       </c>
       <c r="C46" t="s">
-        <v>158</v>
+        <v>129</v>
       </c>
       <c r="D46" t="s">
         <v>59</v>
       </c>
       <c r="E46" t="s">
-        <v>159</v>
+        <v>141</v>
       </c>
       <c r="F46" t="b">
         <v>0</v>
       </c>
       <c r="G46" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H46" t="b">
         <v>0</v>
@@ -4204,7 +4412,7 @@
         <v>1</v>
       </c>
       <c r="L46" t="s">
-        <v>150</v>
+        <v>130</v>
       </c>
       <c r="M46" t="b">
         <v>1</v>
@@ -4221,31 +4429,31 @@
       <c r="S46">
         <v>-1</v>
       </c>
-      <c r="T46">
-        <v>-1</v>
+      <c r="T46" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="47" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="B47" t="s">
-        <v>160</v>
+        <v>181</v>
       </c>
       <c r="C47" t="s">
-        <v>153</v>
+        <v>177</v>
       </c>
       <c r="D47" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="E47" t="s">
-        <v>161</v>
+        <v>177</v>
       </c>
       <c r="F47" t="b">
         <v>0</v>
       </c>
       <c r="G47" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H47" t="b">
         <v>0</v>
@@ -4253,49 +4461,61 @@
       <c r="I47" t="b">
         <v>1</v>
       </c>
+      <c r="J47">
+        <v>1</v>
+      </c>
+      <c r="K47">
+        <v>200</v>
+      </c>
       <c r="L47" t="s">
-        <v>154</v>
+        <v>29</v>
       </c>
       <c r="M47" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N47">
-        <v>-1</v>
-      </c>
-      <c r="Q47" t="s">
-        <v>29</v>
-      </c>
-      <c r="R47" t="b">
-        <v>0</v>
-      </c>
-      <c r="S47">
-        <v>-1</v>
-      </c>
-      <c r="T47">
-        <v>-1</v>
+        <v>4000</v>
+      </c>
+      <c r="O47" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="P47" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q47" s="1">
+        <v>0</v>
+      </c>
+      <c r="R47" s="1">
+        <v>0</v>
+      </c>
+      <c r="S47" s="1">
+        <v>0</v>
+      </c>
+      <c r="T47" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="48" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>154</v>
+        <v>134</v>
       </c>
       <c r="B48" t="s">
-        <v>93</v>
+        <v>109</v>
       </c>
       <c r="C48" t="s">
-        <v>12</v>
+        <v>142</v>
       </c>
       <c r="D48" t="s">
         <v>1</v>
       </c>
       <c r="E48" t="s">
-        <v>162</v>
+        <v>143</v>
       </c>
       <c r="F48" t="b">
         <v>1</v>
       </c>
       <c r="G48" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H48" t="b">
         <v>1</v>
@@ -4324,49 +4544,46 @@
       <c r="S48">
         <v>-1</v>
       </c>
-      <c r="T48">
-        <v>-1</v>
+      <c r="T48" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="49" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>164</v>
+        <v>134</v>
       </c>
       <c r="B49" t="s">
-        <v>93</v>
+        <v>137</v>
       </c>
       <c r="C49" t="s">
-        <v>12</v>
+        <v>136</v>
       </c>
       <c r="D49" t="s">
-        <v>1</v>
+        <v>59</v>
       </c>
       <c r="E49" t="s">
-        <v>162</v>
+        <v>144</v>
       </c>
       <c r="F49" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G49" t="b">
         <v>1</v>
       </c>
       <c r="H49" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I49" t="b">
         <v>1</v>
       </c>
       <c r="L49" t="s">
-        <v>29</v>
+        <v>137</v>
       </c>
       <c r="M49" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N49">
-        <v>100</v>
-      </c>
-      <c r="O49" t="s">
-        <v>30</v>
+        <v>-1</v>
       </c>
       <c r="Q49" t="s">
         <v>29</v>
@@ -4377,22 +4594,832 @@
       <c r="S49">
         <v>-1</v>
       </c>
-      <c r="T49">
+      <c r="T49" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>134</v>
+      </c>
+      <c r="B50" t="s">
+        <v>107</v>
+      </c>
+      <c r="C50" t="s">
+        <v>112</v>
+      </c>
+      <c r="D50" t="s">
+        <v>60</v>
+      </c>
+      <c r="F50" t="b">
+        <v>0</v>
+      </c>
+      <c r="G50" t="b">
+        <v>1</v>
+      </c>
+      <c r="H50" t="b">
+        <v>1</v>
+      </c>
+      <c r="I50" t="b">
+        <v>1</v>
+      </c>
+      <c r="L50" t="s">
+        <v>29</v>
+      </c>
+      <c r="M50" t="b">
+        <v>0</v>
+      </c>
+      <c r="N50">
         <v>-1</v>
+      </c>
+      <c r="Q50" t="s">
+        <v>29</v>
+      </c>
+      <c r="R50" t="b">
+        <v>0</v>
+      </c>
+      <c r="S50">
+        <v>-1</v>
+      </c>
+      <c r="T50" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>134</v>
+      </c>
+      <c r="B51" t="s">
+        <v>110</v>
+      </c>
+      <c r="C51" t="s">
+        <v>147</v>
+      </c>
+      <c r="D51" t="s">
+        <v>1</v>
+      </c>
+      <c r="F51" t="b">
+        <v>0</v>
+      </c>
+      <c r="G51" t="b">
+        <v>0</v>
+      </c>
+      <c r="H51" t="b">
+        <v>1</v>
+      </c>
+      <c r="I51" t="b">
+        <v>1</v>
+      </c>
+      <c r="L51" t="s">
+        <v>29</v>
+      </c>
+      <c r="M51" t="b">
+        <v>0</v>
+      </c>
+      <c r="N51">
+        <v>200</v>
+      </c>
+      <c r="O51" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q51" t="s">
+        <v>29</v>
+      </c>
+      <c r="R51" t="b">
+        <v>0</v>
+      </c>
+      <c r="S51">
+        <v>-1</v>
+      </c>
+      <c r="T51">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>134</v>
+      </c>
+      <c r="B52" t="s">
+        <v>108</v>
+      </c>
+      <c r="C52" t="s">
+        <v>113</v>
+      </c>
+      <c r="D52" t="s">
+        <v>1</v>
+      </c>
+      <c r="F52" t="b">
+        <v>0</v>
+      </c>
+      <c r="G52" t="b">
+        <v>0</v>
+      </c>
+      <c r="H52" t="b">
+        <v>1</v>
+      </c>
+      <c r="I52" t="b">
+        <v>1</v>
+      </c>
+      <c r="L52" t="s">
+        <v>29</v>
+      </c>
+      <c r="M52" t="b">
+        <v>0</v>
+      </c>
+      <c r="N52">
+        <v>200</v>
+      </c>
+      <c r="O52" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q52" t="s">
+        <v>29</v>
+      </c>
+      <c r="R52" t="b">
+        <v>0</v>
+      </c>
+      <c r="S52">
+        <v>-1</v>
+      </c>
+      <c r="T52">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>134</v>
+      </c>
+      <c r="B53" t="s">
+        <v>111</v>
+      </c>
+      <c r="C53" t="s">
+        <v>148</v>
+      </c>
+      <c r="D53" t="s">
+        <v>1</v>
+      </c>
+      <c r="F53" t="b">
+        <v>0</v>
+      </c>
+      <c r="G53" t="b">
+        <v>0</v>
+      </c>
+      <c r="H53" t="b">
+        <v>1</v>
+      </c>
+      <c r="I53" t="b">
+        <v>1</v>
+      </c>
+      <c r="L53" t="s">
+        <v>29</v>
+      </c>
+      <c r="M53" t="b">
+        <v>0</v>
+      </c>
+      <c r="N53">
+        <v>150</v>
+      </c>
+      <c r="O53" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q53" t="s">
+        <v>29</v>
+      </c>
+      <c r="R53" t="b">
+        <v>0</v>
+      </c>
+      <c r="S53">
+        <v>-1</v>
+      </c>
+      <c r="T53">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>150</v>
+      </c>
+      <c r="B54" t="s">
+        <v>93</v>
+      </c>
+      <c r="C54" t="s">
+        <v>12</v>
+      </c>
+      <c r="D54" t="s">
+        <v>1</v>
+      </c>
+      <c r="E54" t="s">
+        <v>162</v>
+      </c>
+      <c r="F54" t="b">
+        <v>1</v>
+      </c>
+      <c r="G54" t="b">
+        <v>1</v>
+      </c>
+      <c r="H54" t="b">
+        <v>1</v>
+      </c>
+      <c r="I54" t="b">
+        <v>1</v>
+      </c>
+      <c r="L54" t="s">
+        <v>29</v>
+      </c>
+      <c r="M54" t="b">
+        <v>0</v>
+      </c>
+      <c r="N54">
+        <v>100</v>
+      </c>
+      <c r="O54" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q54" t="s">
+        <v>29</v>
+      </c>
+      <c r="R54" t="b">
+        <v>0</v>
+      </c>
+      <c r="S54">
+        <v>-1</v>
+      </c>
+      <c r="T54">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>150</v>
+      </c>
+      <c r="B55" t="s">
+        <v>157</v>
+      </c>
+      <c r="C55" t="s">
+        <v>158</v>
+      </c>
+      <c r="D55" t="s">
+        <v>59</v>
+      </c>
+      <c r="E55" t="s">
+        <v>159</v>
+      </c>
+      <c r="F55" t="b">
+        <v>0</v>
+      </c>
+      <c r="G55" t="b">
+        <v>0</v>
+      </c>
+      <c r="H55" t="b">
+        <v>0</v>
+      </c>
+      <c r="I55" t="b">
+        <v>1</v>
+      </c>
+      <c r="L55" t="s">
+        <v>150</v>
+      </c>
+      <c r="M55" t="b">
+        <v>1</v>
+      </c>
+      <c r="N55">
+        <v>-1</v>
+      </c>
+      <c r="Q55" t="s">
+        <v>29</v>
+      </c>
+      <c r="R55" t="b">
+        <v>0</v>
+      </c>
+      <c r="S55">
+        <v>-1</v>
+      </c>
+      <c r="T55">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>150</v>
+      </c>
+      <c r="B56" t="s">
+        <v>160</v>
+      </c>
+      <c r="C56" t="s">
+        <v>153</v>
+      </c>
+      <c r="D56" t="s">
+        <v>59</v>
+      </c>
+      <c r="E56" t="s">
+        <v>161</v>
+      </c>
+      <c r="F56" t="b">
+        <v>0</v>
+      </c>
+      <c r="G56" t="b">
+        <v>1</v>
+      </c>
+      <c r="H56" t="b">
+        <v>0</v>
+      </c>
+      <c r="I56" t="b">
+        <v>1</v>
+      </c>
+      <c r="L56" t="s">
+        <v>154</v>
+      </c>
+      <c r="M56" t="b">
+        <v>1</v>
+      </c>
+      <c r="N56">
+        <v>-1</v>
+      </c>
+      <c r="Q56" t="s">
+        <v>29</v>
+      </c>
+      <c r="R56" t="b">
+        <v>0</v>
+      </c>
+      <c r="S56">
+        <v>-1</v>
+      </c>
+      <c r="T56">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>154</v>
+      </c>
+      <c r="B57" t="s">
+        <v>93</v>
+      </c>
+      <c r="C57" t="s">
+        <v>12</v>
+      </c>
+      <c r="D57" t="s">
+        <v>1</v>
+      </c>
+      <c r="E57" t="s">
+        <v>162</v>
+      </c>
+      <c r="F57" t="b">
+        <v>1</v>
+      </c>
+      <c r="G57" t="b">
+        <v>1</v>
+      </c>
+      <c r="H57" t="b">
+        <v>1</v>
+      </c>
+      <c r="I57" t="b">
+        <v>1</v>
+      </c>
+      <c r="L57" t="s">
+        <v>29</v>
+      </c>
+      <c r="M57" t="b">
+        <v>0</v>
+      </c>
+      <c r="N57">
+        <v>100</v>
+      </c>
+      <c r="O57" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q57" t="s">
+        <v>29</v>
+      </c>
+      <c r="R57" t="b">
+        <v>0</v>
+      </c>
+      <c r="S57">
+        <v>-1</v>
+      </c>
+      <c r="T57">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>164</v>
+      </c>
+      <c r="B58" t="s">
+        <v>93</v>
+      </c>
+      <c r="C58" t="s">
+        <v>12</v>
+      </c>
+      <c r="D58" t="s">
+        <v>1</v>
+      </c>
+      <c r="E58" t="s">
+        <v>162</v>
+      </c>
+      <c r="F58" t="b">
+        <v>1</v>
+      </c>
+      <c r="G58" t="b">
+        <v>1</v>
+      </c>
+      <c r="H58" t="b">
+        <v>1</v>
+      </c>
+      <c r="I58" t="b">
+        <v>1</v>
+      </c>
+      <c r="L58" t="s">
+        <v>29</v>
+      </c>
+      <c r="M58" t="b">
+        <v>0</v>
+      </c>
+      <c r="N58">
+        <v>100</v>
+      </c>
+      <c r="O58" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q58" t="s">
+        <v>29</v>
+      </c>
+      <c r="R58" t="b">
+        <v>0</v>
+      </c>
+      <c r="S58">
+        <v>-1</v>
+      </c>
+      <c r="T58">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>168</v>
+      </c>
+      <c r="B59" t="s">
+        <v>93</v>
+      </c>
+      <c r="C59" t="s">
+        <v>12</v>
+      </c>
+      <c r="D59" t="s">
+        <v>1</v>
+      </c>
+      <c r="E59" t="s">
+        <v>162</v>
+      </c>
+      <c r="F59" t="b">
+        <v>1</v>
+      </c>
+      <c r="G59" t="b">
+        <v>1</v>
+      </c>
+      <c r="H59" t="b">
+        <v>1</v>
+      </c>
+      <c r="I59" t="b">
+        <v>1</v>
+      </c>
+      <c r="L59" t="s">
+        <v>29</v>
+      </c>
+      <c r="M59" t="b">
+        <v>0</v>
+      </c>
+      <c r="N59">
+        <v>100</v>
+      </c>
+      <c r="O59" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q59" t="s">
+        <v>29</v>
+      </c>
+      <c r="R59" t="b">
+        <v>0</v>
+      </c>
+      <c r="S59">
+        <v>-1</v>
+      </c>
+      <c r="T59">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>168</v>
+      </c>
+      <c r="B60" t="s">
+        <v>167</v>
+      </c>
+      <c r="C60" t="s">
+        <v>163</v>
+      </c>
+      <c r="D60" t="s">
+        <v>59</v>
+      </c>
+      <c r="E60" t="s">
+        <v>163</v>
+      </c>
+      <c r="F60" t="b">
+        <v>0</v>
+      </c>
+      <c r="G60" t="b">
+        <v>0</v>
+      </c>
+      <c r="H60" t="b">
+        <v>0</v>
+      </c>
+      <c r="I60" t="b">
+        <v>1</v>
+      </c>
+      <c r="J60">
+        <v>1</v>
+      </c>
+      <c r="K60">
+        <v>200</v>
+      </c>
+      <c r="L60" t="s">
+        <v>164</v>
+      </c>
+      <c r="M60" t="b">
+        <v>1</v>
+      </c>
+      <c r="N60">
+        <v>202</v>
+      </c>
+      <c r="O60" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="P60" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q60" s="1">
+        <v>-100000000</v>
+      </c>
+      <c r="R60" s="1">
+        <v>100000000</v>
+      </c>
+      <c r="S60" s="1">
+        <v>0</v>
+      </c>
+      <c r="T60" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="61" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>168</v>
+      </c>
+      <c r="B61" t="s">
+        <v>180</v>
+      </c>
+      <c r="C61" t="s">
+        <v>87</v>
+      </c>
+      <c r="D61" t="s">
+        <v>69</v>
+      </c>
+      <c r="E61" t="s">
+        <v>87</v>
+      </c>
+      <c r="F61" t="b">
+        <v>0</v>
+      </c>
+      <c r="G61" t="b">
+        <v>0</v>
+      </c>
+      <c r="H61" t="b">
+        <v>0</v>
+      </c>
+      <c r="I61" t="b">
+        <v>1</v>
+      </c>
+      <c r="J61">
+        <v>1</v>
+      </c>
+      <c r="K61">
+        <v>200</v>
+      </c>
+      <c r="L61" t="s">
+        <v>29</v>
+      </c>
+      <c r="M61" t="b">
+        <v>0</v>
+      </c>
+      <c r="N61">
+        <v>4000</v>
+      </c>
+      <c r="O61" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="P61" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q61" s="1">
+        <v>0</v>
+      </c>
+      <c r="R61" s="1">
+        <v>0</v>
+      </c>
+      <c r="S61" s="1">
+        <v>0</v>
+      </c>
+      <c r="T61" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="62" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>172</v>
+      </c>
+      <c r="B62" t="s">
+        <v>93</v>
+      </c>
+      <c r="C62" t="s">
+        <v>12</v>
+      </c>
+      <c r="D62" t="s">
+        <v>1</v>
+      </c>
+      <c r="E62" t="s">
+        <v>162</v>
+      </c>
+      <c r="F62" t="b">
+        <v>1</v>
+      </c>
+      <c r="G62" t="b">
+        <v>1</v>
+      </c>
+      <c r="H62" t="b">
+        <v>1</v>
+      </c>
+      <c r="I62" t="b">
+        <v>1</v>
+      </c>
+      <c r="L62" t="s">
+        <v>29</v>
+      </c>
+      <c r="M62" t="b">
+        <v>0</v>
+      </c>
+      <c r="N62">
+        <v>100</v>
+      </c>
+      <c r="O62" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q62" t="s">
+        <v>29</v>
+      </c>
+      <c r="R62" t="b">
+        <v>0</v>
+      </c>
+      <c r="S62">
+        <v>-1</v>
+      </c>
+      <c r="T62">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>172</v>
+      </c>
+      <c r="B63" t="s">
+        <v>167</v>
+      </c>
+      <c r="C63" t="s">
+        <v>163</v>
+      </c>
+      <c r="D63" t="s">
+        <v>59</v>
+      </c>
+      <c r="E63" t="s">
+        <v>163</v>
+      </c>
+      <c r="F63" t="b">
+        <v>0</v>
+      </c>
+      <c r="G63" t="b">
+        <v>0</v>
+      </c>
+      <c r="H63" t="b">
+        <v>0</v>
+      </c>
+      <c r="I63" t="b">
+        <v>1</v>
+      </c>
+      <c r="J63">
+        <v>1</v>
+      </c>
+      <c r="K63">
+        <v>200</v>
+      </c>
+      <c r="L63" t="s">
+        <v>164</v>
+      </c>
+      <c r="M63" t="b">
+        <v>1</v>
+      </c>
+      <c r="N63">
+        <v>202</v>
+      </c>
+      <c r="O63" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="P63" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q63" s="1">
+        <v>-100000000</v>
+      </c>
+      <c r="R63" s="1">
+        <v>100000000</v>
+      </c>
+      <c r="S63" s="1">
+        <v>0</v>
+      </c>
+      <c r="T63" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>172</v>
+      </c>
+      <c r="B64" t="s">
+        <v>181</v>
+      </c>
+      <c r="C64" t="s">
+        <v>177</v>
+      </c>
+      <c r="D64" t="s">
+        <v>69</v>
+      </c>
+      <c r="E64" t="s">
+        <v>177</v>
+      </c>
+      <c r="F64" t="b">
+        <v>0</v>
+      </c>
+      <c r="G64" t="b">
+        <v>0</v>
+      </c>
+      <c r="H64" t="b">
+        <v>0</v>
+      </c>
+      <c r="I64" t="b">
+        <v>1</v>
+      </c>
+      <c r="J64">
+        <v>1</v>
+      </c>
+      <c r="K64">
+        <v>200</v>
+      </c>
+      <c r="L64" t="s">
+        <v>29</v>
+      </c>
+      <c r="M64" t="b">
+        <v>0</v>
+      </c>
+      <c r="N64">
+        <v>4000</v>
+      </c>
+      <c r="O64" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="P64" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q64" s="1">
+        <v>0</v>
+      </c>
+      <c r="R64" s="1">
+        <v>0</v>
+      </c>
+      <c r="S64" s="1">
+        <v>0</v>
+      </c>
+      <c r="T64" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D7 D16:D19 D25:D27 D30:D65536">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D7 D16:D19 D37:D65546 D26:D32 D21 D34:D35">
       <formula1>"Boolean,Date,Decimal,Double,Integer,Lookup,Money,Picklist,String,Memo,Status"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2:O19 O25:O27 O30:O65536">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2:O19 O37:O65546 O26:O32 O21 O34:O35">
       <formula1>"Text,TextArea,Email,Url,TickerSymbol,Phone"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt=" - " sqref="O20:O24 O28:O29">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt=" - " sqref="O36 O33 O20 O22:O25">
       <formula1>"Text,TextArea,Email,Url,TickerSymbol,Phone"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt=" - " sqref="D20:D24 D28:D29">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt=" - " sqref="D36 D33 D20 D22:D25">
       <formula1>"Boolean,Customer,Date,Decimal,Double,Integer,Lookup,Money,Picklist,String,Memo,Status"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Add associated records to those included when adding modified portal records into release or data export/migration
</commit_message>
<xml_diff>
--- a/SolutionItems/Customisations.xlsx
+++ b/SolutionItems/Customisations.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="120" yWindow="120" windowWidth="23820" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="23820" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Record Types" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="670" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="763" uniqueCount="206">
   <si>
     <t>Relationship Name</t>
   </si>
@@ -568,13 +568,85 @@
   </si>
   <si>
     <t>adx_registerstartupscript</t>
+  </si>
+  <si>
+    <t>adx_contentsnippet</t>
+  </si>
+  <si>
+    <t>adx_entitypermission</t>
+  </si>
+  <si>
+    <t>adx_pagetemplate</t>
+  </si>
+  <si>
+    <t>adx_publishingstate</t>
+  </si>
+  <si>
+    <t>adx_sitemarker</t>
+  </si>
+  <si>
+    <t>adx_sitesetting</t>
+  </si>
+  <si>
+    <t>Content Snippet</t>
+  </si>
+  <si>
+    <t>Entity Permission</t>
+  </si>
+  <si>
+    <t>Page Template</t>
+  </si>
+  <si>
+    <t>Site Marker</t>
+  </si>
+  <si>
+    <t>Site Setting</t>
+  </si>
+  <si>
+    <t>Publishing State</t>
+  </si>
+  <si>
+    <t>Entity Permissions</t>
+  </si>
+  <si>
+    <t>Page Templates</t>
+  </si>
+  <si>
+    <t>Publishing States</t>
+  </si>
+  <si>
+    <t>Site Markers</t>
+  </si>
+  <si>
+    <t>Site Settings</t>
+  </si>
+  <si>
+    <t>Content Snippets</t>
+  </si>
+  <si>
+    <t>adx_contentaccesslevel</t>
+  </si>
+  <si>
+    <t>Content Access Level</t>
+  </si>
+  <si>
+    <t>Content Access Levels</t>
+  </si>
+  <si>
+    <t>adx_entitypermission_webrole</t>
+  </si>
+  <si>
+    <t>adx_WebRoleContentAccessLevel</t>
+  </si>
+  <si>
+    <t>adx_accesscontrolrule_publishingstate</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -595,6 +667,12 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -617,12 +695,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -927,10 +1006,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K19"/>
+  <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1607,6 +1686,251 @@
         <v>0</v>
       </c>
     </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>188</v>
+      </c>
+      <c r="B20" t="s">
+        <v>182</v>
+      </c>
+      <c r="C20" t="s">
+        <v>199</v>
+      </c>
+      <c r="D20" t="s">
+        <v>199</v>
+      </c>
+      <c r="E20" t="b">
+        <v>0</v>
+      </c>
+      <c r="F20" t="b">
+        <v>0</v>
+      </c>
+      <c r="G20" t="b">
+        <v>1</v>
+      </c>
+      <c r="H20" t="b">
+        <v>1</v>
+      </c>
+      <c r="I20" t="b">
+        <v>1</v>
+      </c>
+      <c r="J20" t="b">
+        <v>1</v>
+      </c>
+      <c r="K20" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>189</v>
+      </c>
+      <c r="B21" t="s">
+        <v>183</v>
+      </c>
+      <c r="C21" t="s">
+        <v>194</v>
+      </c>
+      <c r="D21" t="s">
+        <v>194</v>
+      </c>
+      <c r="E21" t="b">
+        <v>0</v>
+      </c>
+      <c r="F21" t="b">
+        <v>0</v>
+      </c>
+      <c r="G21" t="b">
+        <v>1</v>
+      </c>
+      <c r="H21" t="b">
+        <v>1</v>
+      </c>
+      <c r="I21" t="b">
+        <v>1</v>
+      </c>
+      <c r="J21" t="b">
+        <v>1</v>
+      </c>
+      <c r="K21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>190</v>
+      </c>
+      <c r="B22" t="s">
+        <v>184</v>
+      </c>
+      <c r="C22" t="s">
+        <v>195</v>
+      </c>
+      <c r="D22" t="s">
+        <v>195</v>
+      </c>
+      <c r="E22" t="b">
+        <v>0</v>
+      </c>
+      <c r="F22" t="b">
+        <v>0</v>
+      </c>
+      <c r="G22" t="b">
+        <v>1</v>
+      </c>
+      <c r="H22" t="b">
+        <v>1</v>
+      </c>
+      <c r="I22" t="b">
+        <v>1</v>
+      </c>
+      <c r="J22" t="b">
+        <v>1</v>
+      </c>
+      <c r="K22" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>193</v>
+      </c>
+      <c r="B23" t="s">
+        <v>185</v>
+      </c>
+      <c r="C23" t="s">
+        <v>196</v>
+      </c>
+      <c r="D23" t="s">
+        <v>196</v>
+      </c>
+      <c r="E23" t="b">
+        <v>0</v>
+      </c>
+      <c r="F23" t="b">
+        <v>0</v>
+      </c>
+      <c r="G23" t="b">
+        <v>1</v>
+      </c>
+      <c r="H23" t="b">
+        <v>1</v>
+      </c>
+      <c r="I23" t="b">
+        <v>1</v>
+      </c>
+      <c r="J23" t="b">
+        <v>1</v>
+      </c>
+      <c r="K23" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>191</v>
+      </c>
+      <c r="B24" t="s">
+        <v>186</v>
+      </c>
+      <c r="C24" t="s">
+        <v>197</v>
+      </c>
+      <c r="D24" t="s">
+        <v>197</v>
+      </c>
+      <c r="E24" t="b">
+        <v>0</v>
+      </c>
+      <c r="F24" t="b">
+        <v>0</v>
+      </c>
+      <c r="G24" t="b">
+        <v>1</v>
+      </c>
+      <c r="H24" t="b">
+        <v>1</v>
+      </c>
+      <c r="I24" t="b">
+        <v>1</v>
+      </c>
+      <c r="J24" t="b">
+        <v>1</v>
+      </c>
+      <c r="K24" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>192</v>
+      </c>
+      <c r="B25" t="s">
+        <v>187</v>
+      </c>
+      <c r="C25" t="s">
+        <v>198</v>
+      </c>
+      <c r="D25" t="s">
+        <v>198</v>
+      </c>
+      <c r="E25" t="b">
+        <v>0</v>
+      </c>
+      <c r="F25" t="b">
+        <v>0</v>
+      </c>
+      <c r="G25" t="b">
+        <v>1</v>
+      </c>
+      <c r="H25" t="b">
+        <v>1</v>
+      </c>
+      <c r="I25" t="b">
+        <v>1</v>
+      </c>
+      <c r="J25" t="b">
+        <v>1</v>
+      </c>
+      <c r="K25" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>201</v>
+      </c>
+      <c r="B26" t="s">
+        <v>200</v>
+      </c>
+      <c r="C26" t="s">
+        <v>202</v>
+      </c>
+      <c r="D26" t="s">
+        <v>202</v>
+      </c>
+      <c r="E26" t="b">
+        <v>0</v>
+      </c>
+      <c r="F26" t="b">
+        <v>0</v>
+      </c>
+      <c r="G26" t="b">
+        <v>1</v>
+      </c>
+      <c r="H26" t="b">
+        <v>1</v>
+      </c>
+      <c r="I26" t="b">
+        <v>1</v>
+      </c>
+      <c r="J26" t="b">
+        <v>1</v>
+      </c>
+      <c r="K26" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1615,10 +1939,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T64"/>
+  <dimension ref="A1:T71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="I74" sqref="A71:I74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1627,7 +1951,8 @@
     <col min="2" max="2" width="25.5703125" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
     <col min="4" max="4" width="15.5703125" customWidth="1"/>
-    <col min="5" max="6" width="24" customWidth="1"/>
+    <col min="5" max="5" width="41.28515625" customWidth="1"/>
+    <col min="6" max="6" width="24" customWidth="1"/>
     <col min="7" max="7" width="13.140625" customWidth="1"/>
     <col min="8" max="8" width="8.140625" customWidth="1"/>
     <col min="9" max="11" width="12.28515625" customWidth="1"/>
@@ -5408,12 +5733,383 @@
         <v>29</v>
       </c>
     </row>
+    <row r="65" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>182</v>
+      </c>
+      <c r="B65" t="s">
+        <v>93</v>
+      </c>
+      <c r="C65" t="s">
+        <v>12</v>
+      </c>
+      <c r="D65" t="s">
+        <v>1</v>
+      </c>
+      <c r="E65" t="s">
+        <v>162</v>
+      </c>
+      <c r="F65" t="b">
+        <v>1</v>
+      </c>
+      <c r="G65" t="b">
+        <v>1</v>
+      </c>
+      <c r="H65" t="b">
+        <v>1</v>
+      </c>
+      <c r="I65" t="b">
+        <v>1</v>
+      </c>
+      <c r="L65" t="s">
+        <v>29</v>
+      </c>
+      <c r="M65" t="b">
+        <v>0</v>
+      </c>
+      <c r="N65">
+        <v>100</v>
+      </c>
+      <c r="O65" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q65" t="s">
+        <v>29</v>
+      </c>
+      <c r="R65" t="b">
+        <v>0</v>
+      </c>
+      <c r="S65">
+        <v>-1</v>
+      </c>
+      <c r="T65">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>183</v>
+      </c>
+      <c r="B66" t="s">
+        <v>93</v>
+      </c>
+      <c r="C66" t="s">
+        <v>12</v>
+      </c>
+      <c r="D66" t="s">
+        <v>1</v>
+      </c>
+      <c r="E66" t="s">
+        <v>162</v>
+      </c>
+      <c r="F66" t="b">
+        <v>1</v>
+      </c>
+      <c r="G66" t="b">
+        <v>1</v>
+      </c>
+      <c r="H66" t="b">
+        <v>1</v>
+      </c>
+      <c r="I66" t="b">
+        <v>1</v>
+      </c>
+      <c r="L66" t="s">
+        <v>29</v>
+      </c>
+      <c r="M66" t="b">
+        <v>0</v>
+      </c>
+      <c r="N66">
+        <v>100</v>
+      </c>
+      <c r="O66" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q66" t="s">
+        <v>29</v>
+      </c>
+      <c r="R66" t="b">
+        <v>0</v>
+      </c>
+      <c r="S66">
+        <v>-1</v>
+      </c>
+      <c r="T66">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>184</v>
+      </c>
+      <c r="B67" t="s">
+        <v>93</v>
+      </c>
+      <c r="C67" t="s">
+        <v>12</v>
+      </c>
+      <c r="D67" t="s">
+        <v>1</v>
+      </c>
+      <c r="E67" t="s">
+        <v>162</v>
+      </c>
+      <c r="F67" t="b">
+        <v>1</v>
+      </c>
+      <c r="G67" t="b">
+        <v>1</v>
+      </c>
+      <c r="H67" t="b">
+        <v>1</v>
+      </c>
+      <c r="I67" t="b">
+        <v>1</v>
+      </c>
+      <c r="L67" t="s">
+        <v>29</v>
+      </c>
+      <c r="M67" t="b">
+        <v>0</v>
+      </c>
+      <c r="N67">
+        <v>100</v>
+      </c>
+      <c r="O67" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q67" t="s">
+        <v>29</v>
+      </c>
+      <c r="R67" t="b">
+        <v>0</v>
+      </c>
+      <c r="S67">
+        <v>-1</v>
+      </c>
+      <c r="T67">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>185</v>
+      </c>
+      <c r="B68" t="s">
+        <v>93</v>
+      </c>
+      <c r="C68" t="s">
+        <v>12</v>
+      </c>
+      <c r="D68" t="s">
+        <v>1</v>
+      </c>
+      <c r="E68" t="s">
+        <v>162</v>
+      </c>
+      <c r="F68" t="b">
+        <v>1</v>
+      </c>
+      <c r="G68" t="b">
+        <v>1</v>
+      </c>
+      <c r="H68" t="b">
+        <v>1</v>
+      </c>
+      <c r="I68" t="b">
+        <v>1</v>
+      </c>
+      <c r="L68" t="s">
+        <v>29</v>
+      </c>
+      <c r="M68" t="b">
+        <v>0</v>
+      </c>
+      <c r="N68">
+        <v>100</v>
+      </c>
+      <c r="O68" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q68" t="s">
+        <v>29</v>
+      </c>
+      <c r="R68" t="b">
+        <v>0</v>
+      </c>
+      <c r="S68">
+        <v>-1</v>
+      </c>
+      <c r="T68">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>186</v>
+      </c>
+      <c r="B69" t="s">
+        <v>93</v>
+      </c>
+      <c r="C69" t="s">
+        <v>12</v>
+      </c>
+      <c r="D69" t="s">
+        <v>1</v>
+      </c>
+      <c r="E69" t="s">
+        <v>162</v>
+      </c>
+      <c r="F69" t="b">
+        <v>1</v>
+      </c>
+      <c r="G69" t="b">
+        <v>1</v>
+      </c>
+      <c r="H69" t="b">
+        <v>1</v>
+      </c>
+      <c r="I69" t="b">
+        <v>1</v>
+      </c>
+      <c r="L69" t="s">
+        <v>29</v>
+      </c>
+      <c r="M69" t="b">
+        <v>0</v>
+      </c>
+      <c r="N69">
+        <v>100</v>
+      </c>
+      <c r="O69" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q69" t="s">
+        <v>29</v>
+      </c>
+      <c r="R69" t="b">
+        <v>0</v>
+      </c>
+      <c r="S69">
+        <v>-1</v>
+      </c>
+      <c r="T69">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>187</v>
+      </c>
+      <c r="B70" t="s">
+        <v>93</v>
+      </c>
+      <c r="C70" t="s">
+        <v>12</v>
+      </c>
+      <c r="D70" t="s">
+        <v>1</v>
+      </c>
+      <c r="E70" t="s">
+        <v>162</v>
+      </c>
+      <c r="F70" t="b">
+        <v>1</v>
+      </c>
+      <c r="G70" t="b">
+        <v>1</v>
+      </c>
+      <c r="H70" t="b">
+        <v>1</v>
+      </c>
+      <c r="I70" t="b">
+        <v>1</v>
+      </c>
+      <c r="L70" t="s">
+        <v>29</v>
+      </c>
+      <c r="M70" t="b">
+        <v>0</v>
+      </c>
+      <c r="N70">
+        <v>100</v>
+      </c>
+      <c r="O70" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q70" t="s">
+        <v>29</v>
+      </c>
+      <c r="R70" t="b">
+        <v>0</v>
+      </c>
+      <c r="S70">
+        <v>-1</v>
+      </c>
+      <c r="T70">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>200</v>
+      </c>
+      <c r="B71" t="s">
+        <v>93</v>
+      </c>
+      <c r="C71" t="s">
+        <v>12</v>
+      </c>
+      <c r="D71" t="s">
+        <v>1</v>
+      </c>
+      <c r="E71" t="s">
+        <v>162</v>
+      </c>
+      <c r="F71" t="b">
+        <v>1</v>
+      </c>
+      <c r="G71" t="b">
+        <v>1</v>
+      </c>
+      <c r="H71" t="b">
+        <v>1</v>
+      </c>
+      <c r="I71" t="b">
+        <v>1</v>
+      </c>
+      <c r="L71" t="s">
+        <v>29</v>
+      </c>
+      <c r="M71" t="b">
+        <v>0</v>
+      </c>
+      <c r="N71">
+        <v>101</v>
+      </c>
+      <c r="O71" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q71" t="s">
+        <v>29</v>
+      </c>
+      <c r="R71" t="b">
+        <v>0</v>
+      </c>
+      <c r="S71">
+        <v>-1</v>
+      </c>
+      <c r="T71">
+        <v>-1</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D7 D16:D19 D37:D65546 D26:D32 D21 D34:D35">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D7 D16:D19 D34:D35 D26:D32 D21 D37:D65546">
       <formula1>"Boolean,Date,Decimal,Double,Integer,Lookup,Money,Picklist,String,Memo,Status"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2:O19 O37:O65546 O26:O32 O21 O34:O35">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2:O19 O34:O35 O26:O32 O21 O37:O65546">
       <formula1>"Text,TextArea,Email,Url,TickerSymbol,Phone"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt=" - " sqref="O36 O33 O20 O22:O25">
@@ -5742,17 +6438,17 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.28515625" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="48.140625" customWidth="1"/>
+    <col min="2" max="2" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31.28515625" customWidth="1"/>
     <col min="5" max="5" width="29.140625" customWidth="1"/>
     <col min="6" max="6" width="18.28515625" customWidth="1"/>
@@ -5881,7 +6577,95 @@
         <v>10000</v>
       </c>
     </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="B5" t="s">
+        <v>183</v>
+      </c>
+      <c r="C5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F5" t="b">
+        <v>0</v>
+      </c>
+      <c r="G5" t="b">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>10000</v>
+      </c>
+      <c r="K5">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="B6" t="s">
+        <v>200</v>
+      </c>
+      <c r="C6" t="s">
+        <v>96</v>
+      </c>
+      <c r="D6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F6" t="b">
+        <v>0</v>
+      </c>
+      <c r="G6" t="b">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>10000</v>
+      </c>
+      <c r="K6">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="B7" t="s">
+        <v>97</v>
+      </c>
+      <c r="C7" t="s">
+        <v>185</v>
+      </c>
+      <c r="D7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G7" t="b">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>10000</v>
+      </c>
+      <c r="K7">
+        <v>10000</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Issue #146 implement import of portal configuration data where mutliple sites
</commit_message>
<xml_diff>
--- a/SolutionItems/Customisations.xlsx
+++ b/SolutionItems/Customisations.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="23820" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="23820" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Record Types" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="763" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="827" uniqueCount="206">
   <si>
     <t>Relationship Name</t>
   </si>
@@ -1939,10 +1939,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T71"/>
+  <dimension ref="A1:T79"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="I74" sqref="A71:I74"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="I59" sqref="I59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6104,12 +6104,508 @@
         <v>-1</v>
       </c>
     </row>
+    <row r="72" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>154</v>
+      </c>
+      <c r="B72" t="s">
+        <v>167</v>
+      </c>
+      <c r="C72" t="s">
+        <v>163</v>
+      </c>
+      <c r="D72" t="s">
+        <v>59</v>
+      </c>
+      <c r="E72" t="s">
+        <v>163</v>
+      </c>
+      <c r="F72" t="b">
+        <v>0</v>
+      </c>
+      <c r="G72" t="b">
+        <v>0</v>
+      </c>
+      <c r="H72" t="b">
+        <v>0</v>
+      </c>
+      <c r="I72" t="b">
+        <v>1</v>
+      </c>
+      <c r="J72">
+        <v>1</v>
+      </c>
+      <c r="K72">
+        <v>200</v>
+      </c>
+      <c r="L72" t="s">
+        <v>164</v>
+      </c>
+      <c r="M72" t="b">
+        <v>1</v>
+      </c>
+      <c r="N72">
+        <v>202</v>
+      </c>
+      <c r="O72" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="P72" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q72" s="1">
+        <v>-100000000</v>
+      </c>
+      <c r="R72" s="1">
+        <v>100000000</v>
+      </c>
+      <c r="S72" s="1">
+        <v>0</v>
+      </c>
+      <c r="T72" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="73" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>96</v>
+      </c>
+      <c r="B73" t="s">
+        <v>167</v>
+      </c>
+      <c r="C73" t="s">
+        <v>163</v>
+      </c>
+      <c r="D73" t="s">
+        <v>59</v>
+      </c>
+      <c r="E73" t="s">
+        <v>163</v>
+      </c>
+      <c r="F73" t="b">
+        <v>0</v>
+      </c>
+      <c r="G73" t="b">
+        <v>0</v>
+      </c>
+      <c r="H73" t="b">
+        <v>0</v>
+      </c>
+      <c r="I73" t="b">
+        <v>1</v>
+      </c>
+      <c r="J73">
+        <v>1</v>
+      </c>
+      <c r="K73">
+        <v>200</v>
+      </c>
+      <c r="L73" t="s">
+        <v>164</v>
+      </c>
+      <c r="M73" t="b">
+        <v>1</v>
+      </c>
+      <c r="N73">
+        <v>202</v>
+      </c>
+      <c r="O73" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="P73" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q73" s="1">
+        <v>-100000000</v>
+      </c>
+      <c r="R73" s="1">
+        <v>100000000</v>
+      </c>
+      <c r="S73" s="1">
+        <v>0</v>
+      </c>
+      <c r="T73" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="74" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>187</v>
+      </c>
+      <c r="B74" t="s">
+        <v>167</v>
+      </c>
+      <c r="C74" t="s">
+        <v>163</v>
+      </c>
+      <c r="D74" t="s">
+        <v>59</v>
+      </c>
+      <c r="E74" t="s">
+        <v>163</v>
+      </c>
+      <c r="F74" t="b">
+        <v>0</v>
+      </c>
+      <c r="G74" t="b">
+        <v>0</v>
+      </c>
+      <c r="H74" t="b">
+        <v>0</v>
+      </c>
+      <c r="I74" t="b">
+        <v>1</v>
+      </c>
+      <c r="J74">
+        <v>1</v>
+      </c>
+      <c r="K74">
+        <v>200</v>
+      </c>
+      <c r="L74" t="s">
+        <v>164</v>
+      </c>
+      <c r="M74" t="b">
+        <v>1</v>
+      </c>
+      <c r="N74">
+        <v>202</v>
+      </c>
+      <c r="O74" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="P74" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q74" s="1">
+        <v>-100000000</v>
+      </c>
+      <c r="R74" s="1">
+        <v>100000000</v>
+      </c>
+      <c r="S74" s="1">
+        <v>0</v>
+      </c>
+      <c r="T74" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="75" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>186</v>
+      </c>
+      <c r="B75" t="s">
+        <v>167</v>
+      </c>
+      <c r="C75" t="s">
+        <v>163</v>
+      </c>
+      <c r="D75" t="s">
+        <v>59</v>
+      </c>
+      <c r="E75" t="s">
+        <v>163</v>
+      </c>
+      <c r="F75" t="b">
+        <v>0</v>
+      </c>
+      <c r="G75" t="b">
+        <v>0</v>
+      </c>
+      <c r="H75" t="b">
+        <v>0</v>
+      </c>
+      <c r="I75" t="b">
+        <v>1</v>
+      </c>
+      <c r="J75">
+        <v>1</v>
+      </c>
+      <c r="K75">
+        <v>200</v>
+      </c>
+      <c r="L75" t="s">
+        <v>164</v>
+      </c>
+      <c r="M75" t="b">
+        <v>1</v>
+      </c>
+      <c r="N75">
+        <v>202</v>
+      </c>
+      <c r="O75" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="P75" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q75" s="1">
+        <v>-100000000</v>
+      </c>
+      <c r="R75" s="1">
+        <v>100000000</v>
+      </c>
+      <c r="S75" s="1">
+        <v>0</v>
+      </c>
+      <c r="T75" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="76" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>185</v>
+      </c>
+      <c r="B76" t="s">
+        <v>167</v>
+      </c>
+      <c r="C76" t="s">
+        <v>163</v>
+      </c>
+      <c r="D76" t="s">
+        <v>59</v>
+      </c>
+      <c r="E76" t="s">
+        <v>163</v>
+      </c>
+      <c r="F76" t="b">
+        <v>0</v>
+      </c>
+      <c r="G76" t="b">
+        <v>0</v>
+      </c>
+      <c r="H76" t="b">
+        <v>0</v>
+      </c>
+      <c r="I76" t="b">
+        <v>1</v>
+      </c>
+      <c r="J76">
+        <v>1</v>
+      </c>
+      <c r="K76">
+        <v>200</v>
+      </c>
+      <c r="L76" t="s">
+        <v>164</v>
+      </c>
+      <c r="M76" t="b">
+        <v>1</v>
+      </c>
+      <c r="N76">
+        <v>202</v>
+      </c>
+      <c r="O76" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="P76" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q76" s="1">
+        <v>-100000000</v>
+      </c>
+      <c r="R76" s="1">
+        <v>100000000</v>
+      </c>
+      <c r="S76" s="1">
+        <v>0</v>
+      </c>
+      <c r="T76" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="77" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>184</v>
+      </c>
+      <c r="B77" t="s">
+        <v>167</v>
+      </c>
+      <c r="C77" t="s">
+        <v>163</v>
+      </c>
+      <c r="D77" t="s">
+        <v>59</v>
+      </c>
+      <c r="E77" t="s">
+        <v>163</v>
+      </c>
+      <c r="F77" t="b">
+        <v>0</v>
+      </c>
+      <c r="G77" t="b">
+        <v>0</v>
+      </c>
+      <c r="H77" t="b">
+        <v>0</v>
+      </c>
+      <c r="I77" t="b">
+        <v>1</v>
+      </c>
+      <c r="J77">
+        <v>1</v>
+      </c>
+      <c r="K77">
+        <v>200</v>
+      </c>
+      <c r="L77" t="s">
+        <v>164</v>
+      </c>
+      <c r="M77" t="b">
+        <v>1</v>
+      </c>
+      <c r="N77">
+        <v>202</v>
+      </c>
+      <c r="O77" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="P77" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q77" s="1">
+        <v>-100000000</v>
+      </c>
+      <c r="R77" s="1">
+        <v>100000000</v>
+      </c>
+      <c r="S77" s="1">
+        <v>0</v>
+      </c>
+      <c r="T77" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="78" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>183</v>
+      </c>
+      <c r="B78" t="s">
+        <v>167</v>
+      </c>
+      <c r="C78" t="s">
+        <v>163</v>
+      </c>
+      <c r="D78" t="s">
+        <v>59</v>
+      </c>
+      <c r="E78" t="s">
+        <v>163</v>
+      </c>
+      <c r="F78" t="b">
+        <v>0</v>
+      </c>
+      <c r="G78" t="b">
+        <v>0</v>
+      </c>
+      <c r="H78" t="b">
+        <v>0</v>
+      </c>
+      <c r="I78" t="b">
+        <v>1</v>
+      </c>
+      <c r="J78">
+        <v>1</v>
+      </c>
+      <c r="K78">
+        <v>200</v>
+      </c>
+      <c r="L78" t="s">
+        <v>164</v>
+      </c>
+      <c r="M78" t="b">
+        <v>1</v>
+      </c>
+      <c r="N78">
+        <v>202</v>
+      </c>
+      <c r="O78" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="P78" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q78" s="1">
+        <v>-100000000</v>
+      </c>
+      <c r="R78" s="1">
+        <v>100000000</v>
+      </c>
+      <c r="S78" s="1">
+        <v>0</v>
+      </c>
+      <c r="T78" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="79" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>182</v>
+      </c>
+      <c r="B79" t="s">
+        <v>167</v>
+      </c>
+      <c r="C79" t="s">
+        <v>163</v>
+      </c>
+      <c r="D79" t="s">
+        <v>59</v>
+      </c>
+      <c r="E79" t="s">
+        <v>163</v>
+      </c>
+      <c r="F79" t="b">
+        <v>0</v>
+      </c>
+      <c r="G79" t="b">
+        <v>0</v>
+      </c>
+      <c r="H79" t="b">
+        <v>0</v>
+      </c>
+      <c r="I79" t="b">
+        <v>1</v>
+      </c>
+      <c r="J79">
+        <v>1</v>
+      </c>
+      <c r="K79">
+        <v>200</v>
+      </c>
+      <c r="L79" t="s">
+        <v>164</v>
+      </c>
+      <c r="M79" t="b">
+        <v>1</v>
+      </c>
+      <c r="N79">
+        <v>202</v>
+      </c>
+      <c r="O79" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="P79" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q79" s="1">
+        <v>-100000000</v>
+      </c>
+      <c r="R79" s="1">
+        <v>100000000</v>
+      </c>
+      <c r="S79" s="1">
+        <v>0</v>
+      </c>
+      <c r="T79" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D7 D16:D19 D34:D35 D26:D32 D21 D37:D65546">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D7 D16:D19 D34:D35 D26:D32 D21 D37:D65545">
       <formula1>"Boolean,Date,Decimal,Double,Integer,Lookup,Money,Picklist,String,Memo,Status"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2:O19 O34:O35 O26:O32 O21 O37:O65546">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2:O19 O34:O35 O26:O32 O21 O37:O65545">
       <formula1>"Text,TextArea,Email,Url,TickerSymbol,Phone"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt=" - " sqref="O36 O33 O20 O22:O25">
@@ -6440,8 +6936,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Corrected name of primary field in enitty permission entity
</commit_message>
<xml_diff>
--- a/SolutionItems/Customisations.xlsx
+++ b/SolutionItems/Customisations.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="827" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="827" uniqueCount="207">
   <si>
     <t>Relationship Name</t>
   </si>
@@ -640,6 +640,9 @@
   </si>
   <si>
     <t>adx_accesscontrolrule_publishingstate</t>
+  </si>
+  <si>
+    <t>adx_entityname</t>
   </si>
 </sst>
 </file>
@@ -1942,7 +1945,7 @@
   <dimension ref="A1:T79"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="I59" sqref="I59"/>
+      <selection activeCell="B66" sqref="B66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5791,7 +5794,7 @@
         <v>183</v>
       </c>
       <c r="B66" t="s">
-        <v>93</v>
+        <v>206</v>
       </c>
       <c r="C66" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
Add notes = true for test entity in testing customisations excel
</commit_message>
<xml_diff>
--- a/SolutionItems/Customisations.xlsx
+++ b/SolutionItems/Customisations.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="23820" windowHeight="8016" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="23820" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Record Types" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="836" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="837" uniqueCount="210">
   <si>
     <t>Relationship Name</t>
   </si>
@@ -1018,80 +1018,81 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K26"/>
+  <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.88671875" customWidth="1"/>
-    <col min="2" max="2" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23" customWidth="1"/>
-    <col min="5" max="5" width="8.109375" customWidth="1"/>
+    <col min="2" max="2" width="17.88671875" customWidth="1"/>
+    <col min="3" max="3" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23" customWidth="1"/>
+    <col min="6" max="6" width="8.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" t="b">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
         <v>49</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>48</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>50</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>49</v>
       </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
       <c r="F2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G2">
         <v>0</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -1102,25 +1103,28 @@
       <c r="K2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="L2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" t="b">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
         <v>84</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>80</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>82</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>84</v>
       </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
       <c r="F3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -1137,25 +1141,28 @@
       <c r="K3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="L3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" t="b">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
         <v>85</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>81</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>83</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>85</v>
       </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
       <c r="F4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -1172,31 +1179,34 @@
       <c r="K4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" s="3" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+      <c r="L4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" s="3" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" t="b">
+        <v>0</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>92</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>124</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="E5" s="2">
-        <v>1</v>
+      <c r="E5" s="2" t="s">
+        <v>124</v>
       </c>
       <c r="F5" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H5" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I5" s="2">
         <v>0</v>
@@ -1207,25 +1217,28 @@
       <c r="K5" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" s="3" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+      <c r="L5" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" s="3" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" t="b">
+        <v>0</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>94</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>102</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="E6" s="2">
-        <v>1</v>
+      <c r="E6" s="2" t="s">
+        <v>102</v>
       </c>
       <c r="F6" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6" s="2">
         <v>0</v>
@@ -1242,25 +1255,28 @@
       <c r="K6" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" s="3" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+      <c r="L6" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" s="3" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" t="b">
+        <v>0</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>95</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>125</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="E7" s="2">
-        <v>1</v>
+      <c r="E7" s="2" t="s">
+        <v>125</v>
       </c>
       <c r="F7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G7" s="2">
         <v>0</v>
@@ -1277,25 +1293,28 @@
       <c r="K7" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+      <c r="L7" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" t="b">
+        <v>0</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>96</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>126</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="E8" s="2">
-        <v>1</v>
+      <c r="E8" s="2" t="s">
+        <v>126</v>
       </c>
       <c r="F8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G8" s="2">
         <v>0</v>
@@ -1312,25 +1331,28 @@
       <c r="K8" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
+      <c r="L8" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" t="b">
+        <v>0</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>97</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>127</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="E9" s="2">
-        <v>1</v>
+      <c r="E9" s="2" t="s">
+        <v>127</v>
       </c>
       <c r="F9" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G9" s="2">
         <v>0</v>
@@ -1347,25 +1369,28 @@
       <c r="K9" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
+      <c r="L9" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" t="b">
+        <v>0</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>105</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>123</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="E10" s="2">
-        <v>1</v>
+      <c r="E10" s="2" t="s">
+        <v>123</v>
       </c>
       <c r="F10" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G10" s="2">
         <v>0</v>
@@ -1382,25 +1407,28 @@
       <c r="K10" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
+      <c r="L10" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" t="b">
+        <v>0</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>106</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>128</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="E11" s="2">
-        <v>1</v>
+      <c r="E11" s="2" t="s">
+        <v>128</v>
       </c>
       <c r="F11" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G11" s="2">
         <v>0</v>
@@ -1417,23 +1445,26 @@
       <c r="K11" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="L11" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" t="b">
+        <v>0</v>
+      </c>
+      <c r="B12" t="s">
         <v>129</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>130</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>131</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>132</v>
       </c>
-      <c r="E12" t="b">
-        <v>0</v>
-      </c>
       <c r="F12" t="b">
         <v>0</v>
       </c>
@@ -1452,23 +1483,26 @@
       <c r="K12" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="L12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13" t="b">
+        <v>0</v>
+      </c>
+      <c r="B13" t="s">
         <v>133</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>134</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>133</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>135</v>
       </c>
-      <c r="E13" t="b">
-        <v>0</v>
-      </c>
       <c r="F13" t="b">
         <v>0</v>
       </c>
@@ -1487,23 +1521,26 @@
       <c r="K13" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="L13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14" t="b">
+        <v>0</v>
+      </c>
+      <c r="B14" t="s">
         <v>136</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>137</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>138</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>139</v>
       </c>
-      <c r="E14" t="b">
-        <v>0</v>
-      </c>
       <c r="F14" t="b">
         <v>0</v>
       </c>
@@ -1522,58 +1559,64 @@
       <c r="K14" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+      <c r="L14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15" t="b">
+        <v>0</v>
+      </c>
+      <c r="B15" t="s">
         <v>149</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>150</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>151</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>152</v>
       </c>
-      <c r="E15" t="b">
-        <v>0</v>
-      </c>
       <c r="F15" t="b">
         <v>0</v>
       </c>
       <c r="G15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I15" t="b">
         <v>0</v>
       </c>
       <c r="J15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+        <v>1</v>
+      </c>
+      <c r="L15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16" t="b">
+        <v>0</v>
+      </c>
+      <c r="B16" t="s">
         <v>153</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>154</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>155</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>156</v>
       </c>
-      <c r="E16" t="b">
-        <v>0</v>
-      </c>
       <c r="F16" t="b">
         <v>0</v>
       </c>
@@ -1587,33 +1630,36 @@
         <v>0</v>
       </c>
       <c r="J16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K16" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+        <v>1</v>
+      </c>
+      <c r="L16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A17" t="b">
+        <v>0</v>
+      </c>
+      <c r="B17" t="s">
         <v>163</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>164</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>165</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>166</v>
       </c>
-      <c r="E17" t="b">
-        <v>0</v>
-      </c>
       <c r="F17" t="b">
         <v>0</v>
       </c>
       <c r="G17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H17" t="b">
         <v>1</v>
@@ -1625,30 +1671,33 @@
         <v>1</v>
       </c>
       <c r="K17" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+        <v>1</v>
+      </c>
+      <c r="L17" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A18" t="b">
+        <v>0</v>
+      </c>
+      <c r="B18" t="s">
         <v>169</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>168</v>
-      </c>
-      <c r="C18" t="s">
-        <v>170</v>
       </c>
       <c r="D18" t="s">
         <v>170</v>
       </c>
-      <c r="E18" t="b">
-        <v>0</v>
+      <c r="E18" t="s">
+        <v>170</v>
       </c>
       <c r="F18" t="b">
         <v>0</v>
       </c>
       <c r="G18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H18" t="b">
         <v>1</v>
@@ -1660,30 +1709,33 @@
         <v>1</v>
       </c>
       <c r="K18" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+        <v>1</v>
+      </c>
+      <c r="L18" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A19" t="b">
+        <v>0</v>
+      </c>
+      <c r="B19" t="s">
         <v>171</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>172</v>
-      </c>
-      <c r="C19" t="s">
-        <v>173</v>
       </c>
       <c r="D19" t="s">
         <v>173</v>
       </c>
-      <c r="E19" t="b">
-        <v>0</v>
+      <c r="E19" t="s">
+        <v>173</v>
       </c>
       <c r="F19" t="b">
         <v>0</v>
       </c>
       <c r="G19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H19" t="b">
         <v>1</v>
@@ -1695,30 +1747,33 @@
         <v>1</v>
       </c>
       <c r="K19" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+        <v>1</v>
+      </c>
+      <c r="L19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A20" t="b">
+        <v>0</v>
+      </c>
+      <c r="B20" t="s">
         <v>188</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>182</v>
-      </c>
-      <c r="C20" t="s">
-        <v>199</v>
       </c>
       <c r="D20" t="s">
         <v>199</v>
       </c>
-      <c r="E20" t="b">
-        <v>0</v>
+      <c r="E20" t="s">
+        <v>199</v>
       </c>
       <c r="F20" t="b">
         <v>0</v>
       </c>
       <c r="G20" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H20" t="b">
         <v>1</v>
@@ -1730,30 +1785,33 @@
         <v>1</v>
       </c>
       <c r="K20" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+        <v>1</v>
+      </c>
+      <c r="L20" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A21" t="b">
+        <v>0</v>
+      </c>
+      <c r="B21" t="s">
         <v>189</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>183</v>
-      </c>
-      <c r="C21" t="s">
-        <v>194</v>
       </c>
       <c r="D21" t="s">
         <v>194</v>
       </c>
-      <c r="E21" t="b">
-        <v>0</v>
+      <c r="E21" t="s">
+        <v>194</v>
       </c>
       <c r="F21" t="b">
         <v>0</v>
       </c>
       <c r="G21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H21" t="b">
         <v>1</v>
@@ -1765,30 +1823,33 @@
         <v>1</v>
       </c>
       <c r="K21" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+        <v>1</v>
+      </c>
+      <c r="L21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A22" t="b">
+        <v>0</v>
+      </c>
+      <c r="B22" t="s">
         <v>190</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>184</v>
-      </c>
-      <c r="C22" t="s">
-        <v>195</v>
       </c>
       <c r="D22" t="s">
         <v>195</v>
       </c>
-      <c r="E22" t="b">
-        <v>0</v>
+      <c r="E22" t="s">
+        <v>195</v>
       </c>
       <c r="F22" t="b">
         <v>0</v>
       </c>
       <c r="G22" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H22" t="b">
         <v>1</v>
@@ -1800,30 +1861,33 @@
         <v>1</v>
       </c>
       <c r="K22" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+        <v>1</v>
+      </c>
+      <c r="L22" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A23" t="b">
+        <v>0</v>
+      </c>
+      <c r="B23" t="s">
         <v>193</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>185</v>
-      </c>
-      <c r="C23" t="s">
-        <v>196</v>
       </c>
       <c r="D23" t="s">
         <v>196</v>
       </c>
-      <c r="E23" t="b">
-        <v>0</v>
+      <c r="E23" t="s">
+        <v>196</v>
       </c>
       <c r="F23" t="b">
         <v>0</v>
       </c>
       <c r="G23" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H23" t="b">
         <v>1</v>
@@ -1835,30 +1899,33 @@
         <v>1</v>
       </c>
       <c r="K23" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+        <v>1</v>
+      </c>
+      <c r="L23" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A24" t="b">
+        <v>0</v>
+      </c>
+      <c r="B24" t="s">
         <v>191</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>186</v>
-      </c>
-      <c r="C24" t="s">
-        <v>197</v>
       </c>
       <c r="D24" t="s">
         <v>197</v>
       </c>
-      <c r="E24" t="b">
-        <v>0</v>
+      <c r="E24" t="s">
+        <v>197</v>
       </c>
       <c r="F24" t="b">
         <v>0</v>
       </c>
       <c r="G24" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H24" t="b">
         <v>1</v>
@@ -1870,30 +1937,33 @@
         <v>1</v>
       </c>
       <c r="K24" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+        <v>1</v>
+      </c>
+      <c r="L24" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A25" t="b">
+        <v>0</v>
+      </c>
+      <c r="B25" t="s">
         <v>192</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
         <v>187</v>
-      </c>
-      <c r="C25" t="s">
-        <v>198</v>
       </c>
       <c r="D25" t="s">
         <v>198</v>
       </c>
-      <c r="E25" t="b">
-        <v>0</v>
+      <c r="E25" t="s">
+        <v>198</v>
       </c>
       <c r="F25" t="b">
         <v>0</v>
       </c>
       <c r="G25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H25" t="b">
         <v>1</v>
@@ -1905,30 +1975,33 @@
         <v>1</v>
       </c>
       <c r="K25" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+        <v>1</v>
+      </c>
+      <c r="L25" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A26" t="b">
+        <v>0</v>
+      </c>
+      <c r="B26" t="s">
         <v>201</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C26" t="s">
         <v>200</v>
-      </c>
-      <c r="C26" t="s">
-        <v>202</v>
       </c>
       <c r="D26" t="s">
         <v>202</v>
       </c>
-      <c r="E26" t="b">
-        <v>0</v>
+      <c r="E26" t="s">
+        <v>202</v>
       </c>
       <c r="F26" t="b">
         <v>0</v>
       </c>
       <c r="G26" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H26" t="b">
         <v>1</v>
@@ -1940,6 +2013,9 @@
         <v>1</v>
       </c>
       <c r="K26" t="b">
+        <v>1</v>
+      </c>
+      <c r="L26" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1953,8 +2029,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2043,7 +2119,7 @@
     </row>
     <row r="2" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>48</v>
@@ -2108,7 +2184,7 @@
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3" t="s">
         <v>48</v>
@@ -2173,7 +2249,7 @@
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B4" t="s">
         <v>48</v>
@@ -2238,7 +2314,7 @@
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B5" t="s">
         <v>48</v>
@@ -2303,7 +2379,7 @@
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B6" t="s">
         <v>48</v>
@@ -2368,7 +2444,7 @@
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B7" t="s">
         <v>48</v>
@@ -2433,7 +2509,7 @@
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B8" t="s">
         <v>48</v>
@@ -2498,7 +2574,7 @@
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B9" t="s">
         <v>48</v>
@@ -2563,7 +2639,7 @@
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B10" t="s">
         <v>48</v>
@@ -2628,7 +2704,7 @@
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B11" t="s">
         <v>48</v>
@@ -2693,7 +2769,7 @@
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B12" t="s">
         <v>48</v>
@@ -2758,7 +2834,7 @@
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B13" t="s">
         <v>48</v>
@@ -2823,7 +2899,7 @@
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B14" t="s">
         <v>48</v>
@@ -2888,7 +2964,7 @@
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B15" t="s">
         <v>48</v>
@@ -3018,7 +3094,7 @@
     </row>
     <row r="17" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B17" t="s">
         <v>80</v>
@@ -3083,7 +3159,7 @@
     </row>
     <row r="18" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B18" t="s">
         <v>80</v>
@@ -3148,7 +3224,7 @@
     </row>
     <row r="19" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B19" t="s">
         <v>81</v>
@@ -3213,7 +3289,7 @@
     </row>
     <row r="20" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B20" t="s">
         <v>81</v>
@@ -3278,7 +3354,7 @@
     </row>
     <row r="21" spans="1:21" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>92</v>
@@ -3339,7 +3415,7 @@
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>92</v>
@@ -3404,7 +3480,7 @@
     </row>
     <row r="23" spans="1:21" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>94</v>
@@ -3465,7 +3541,7 @@
     </row>
     <row r="24" spans="1:21" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>95</v>
@@ -3526,7 +3602,7 @@
     </row>
     <row r="25" spans="1:21" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>96</v>
@@ -3587,7 +3663,7 @@
     </row>
     <row r="26" spans="1:21" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>97</v>
@@ -3648,7 +3724,7 @@
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>94</v>
@@ -3713,7 +3789,7 @@
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>94</v>
@@ -3778,7 +3854,7 @@
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>94</v>
@@ -3843,7 +3919,7 @@
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>94</v>
@@ -3908,7 +3984,7 @@
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>94</v>
@@ -3973,7 +4049,7 @@
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>94</v>
@@ -4038,7 +4114,7 @@
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>97</v>
@@ -4103,7 +4179,7 @@
     </row>
     <row r="34" spans="1:21" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>105</v>
@@ -4164,7 +4240,7 @@
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>105</v>
@@ -4229,7 +4305,7 @@
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>105</v>
@@ -4294,7 +4370,7 @@
     </row>
     <row r="37" spans="1:21" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>106</v>
@@ -4355,7 +4431,7 @@
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>106</v>
@@ -4420,7 +4496,7 @@
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>106</v>
@@ -4485,7 +4561,7 @@
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>106</v>
@@ -4550,7 +4626,7 @@
     </row>
     <row r="41" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>106</v>
@@ -4615,7 +4691,7 @@
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>106</v>
@@ -4680,7 +4756,7 @@
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>106</v>
@@ -4745,7 +4821,7 @@
     </row>
     <row r="44" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B44" t="s">
         <v>130</v>
@@ -4801,7 +4877,7 @@
     </row>
     <row r="45" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B45" t="s">
         <v>130</v>
@@ -4866,7 +4942,7 @@
     </row>
     <row r="46" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B46" t="s">
         <v>137</v>
@@ -4922,7 +4998,7 @@
     </row>
     <row r="47" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B47" t="s">
         <v>137</v>
@@ -4975,7 +5051,7 @@
     </row>
     <row r="48" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B48" t="s">
         <v>137</v>
@@ -5040,7 +5116,7 @@
     </row>
     <row r="49" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B49" t="s">
         <v>134</v>
@@ -5096,7 +5172,7 @@
     </row>
     <row r="50" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B50" t="s">
         <v>134</v>
@@ -5149,7 +5225,7 @@
     </row>
     <row r="51" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B51" t="s">
         <v>134</v>
@@ -5199,7 +5275,7 @@
     </row>
     <row r="52" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B52" t="s">
         <v>134</v>
@@ -5252,7 +5328,7 @@
     </row>
     <row r="53" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B53" t="s">
         <v>134</v>
@@ -5305,7 +5381,7 @@
     </row>
     <row r="54" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B54" t="s">
         <v>134</v>
@@ -5358,7 +5434,7 @@
     </row>
     <row r="55" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B55" t="s">
         <v>150</v>
@@ -5414,7 +5490,7 @@
     </row>
     <row r="56" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B56" t="s">
         <v>150</v>
@@ -5467,7 +5543,7 @@
     </row>
     <row r="57" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B57" t="s">
         <v>150</v>
@@ -5520,7 +5596,7 @@
     </row>
     <row r="58" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B58" t="s">
         <v>154</v>
@@ -5576,7 +5652,7 @@
     </row>
     <row r="59" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B59" t="s">
         <v>164</v>
@@ -5632,7 +5708,7 @@
     </row>
     <row r="60" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B60" t="s">
         <v>168</v>
@@ -5688,7 +5764,7 @@
     </row>
     <row r="61" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B61" t="s">
         <v>168</v>
@@ -5753,7 +5829,7 @@
     </row>
     <row r="62" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B62" t="s">
         <v>168</v>
@@ -5818,7 +5894,7 @@
     </row>
     <row r="63" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B63" t="s">
         <v>172</v>
@@ -5874,7 +5950,7 @@
     </row>
     <row r="64" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B64" t="s">
         <v>172</v>
@@ -5939,7 +6015,7 @@
     </row>
     <row r="65" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B65" t="s">
         <v>172</v>
@@ -6004,7 +6080,7 @@
     </row>
     <row r="66" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B66" t="s">
         <v>182</v>
@@ -6060,7 +6136,7 @@
     </row>
     <row r="67" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B67" t="s">
         <v>183</v>
@@ -6116,7 +6192,7 @@
     </row>
     <row r="68" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B68" t="s">
         <v>184</v>
@@ -6172,7 +6248,7 @@
     </row>
     <row r="69" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B69" t="s">
         <v>185</v>
@@ -6228,7 +6304,7 @@
     </row>
     <row r="70" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B70" t="s">
         <v>186</v>
@@ -6284,7 +6360,7 @@
     </row>
     <row r="71" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B71" t="s">
         <v>187</v>
@@ -6340,7 +6416,7 @@
     </row>
     <row r="72" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B72" t="s">
         <v>200</v>
@@ -6396,7 +6472,7 @@
     </row>
     <row r="73" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B73" t="s">
         <v>154</v>
@@ -6461,7 +6537,7 @@
     </row>
     <row r="74" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B74" t="s">
         <v>96</v>
@@ -6526,7 +6602,7 @@
     </row>
     <row r="75" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B75" t="s">
         <v>187</v>
@@ -6591,7 +6667,7 @@
     </row>
     <row r="76" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B76" t="s">
         <v>186</v>
@@ -6656,7 +6732,7 @@
     </row>
     <row r="77" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B77" t="s">
         <v>185</v>
@@ -6721,7 +6797,7 @@
     </row>
     <row r="78" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B78" t="s">
         <v>184</v>
@@ -6786,7 +6862,7 @@
     </row>
     <row r="79" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B79" t="s">
         <v>183</v>
@@ -6851,7 +6927,7 @@
     </row>
     <row r="80" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B80" t="s">
         <v>182</v>

</xml_diff>

<commit_message>
Run test scripts & tweak for new online instance
</commit_message>
<xml_diff>
--- a/SolutionItems/Customisations.xlsx
+++ b/SolutionItems/Customisations.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="23820" windowHeight="8016"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="23820" windowHeight="8016" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Record Types" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="837" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="861" uniqueCount="216">
   <si>
     <t>Relationship Name</t>
   </si>
@@ -652,6 +652,24 @@
   </si>
   <si>
     <t>Ignore</t>
+  </si>
+  <si>
+    <t>adx_defaultlanguage</t>
+  </si>
+  <si>
+    <t>Default Language</t>
+  </si>
+  <si>
+    <t>adx_partialurl</t>
+  </si>
+  <si>
+    <t>Partial URL</t>
+  </si>
+  <si>
+    <t>adx_parentpageid</t>
+  </si>
+  <si>
+    <t>Parent Page</t>
   </si>
 </sst>
 </file>
@@ -1020,7 +1038,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2027,10 +2045,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U80"/>
+  <dimension ref="A1:U83"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="C22" workbookViewId="0">
+      <selection activeCell="M34" sqref="M34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4117,19 +4135,19 @@
         <v>0</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C33" t="s">
-        <v>101</v>
+        <v>212</v>
       </c>
       <c r="D33" t="s">
-        <v>102</v>
+        <v>213</v>
       </c>
       <c r="E33" t="s">
-        <v>59</v>
+        <v>1</v>
       </c>
       <c r="F33" t="s">
-        <v>102</v>
+        <v>213</v>
       </c>
       <c r="G33" t="b">
         <v>0</v>
@@ -4149,14 +4167,14 @@
       <c r="L33">
         <v>200</v>
       </c>
-      <c r="M33" s="2" t="s">
-        <v>94</v>
+      <c r="M33" t="s">
+        <v>29</v>
       </c>
       <c r="N33" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O33">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="P33" s="1" t="s">
         <v>30</v>
@@ -4165,10 +4183,10 @@
         <v>0</v>
       </c>
       <c r="R33" s="1">
-        <v>-100000000</v>
+        <v>0</v>
       </c>
       <c r="S33" s="1">
-        <v>100000000</v>
+        <v>0</v>
       </c>
       <c r="T33" s="1">
         <v>0</v>
@@ -4177,63 +4195,67 @@
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="1:21" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="b">
         <v>0</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G34" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="H34" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="I34" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="J34" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="K34" s="2">
-        <v>1</v>
-      </c>
-      <c r="L34" s="2">
-        <v>200</v>
-      </c>
-      <c r="M34" s="2"/>
-      <c r="N34" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="O34" s="2">
-        <v>200</v>
-      </c>
-      <c r="P34" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C34" t="s">
+        <v>214</v>
+      </c>
+      <c r="D34" t="s">
+        <v>215</v>
+      </c>
+      <c r="E34" t="s">
+        <v>59</v>
+      </c>
+      <c r="F34" t="s">
+        <v>215</v>
+      </c>
+      <c r="G34" t="b">
+        <v>0</v>
+      </c>
+      <c r="H34" t="b">
+        <v>0</v>
+      </c>
+      <c r="I34" t="b">
+        <v>0</v>
+      </c>
+      <c r="J34" t="b">
+        <v>1</v>
+      </c>
+      <c r="K34">
+        <v>1</v>
+      </c>
+      <c r="L34">
+        <v>200</v>
+      </c>
+      <c r="M34" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="N34" t="b">
+        <v>0</v>
+      </c>
+      <c r="O34">
+        <v>201</v>
+      </c>
+      <c r="P34" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="Q34" s="4">
-        <v>0</v>
-      </c>
-      <c r="R34" s="4">
-        <v>0</v>
-      </c>
-      <c r="S34" s="4">
-        <v>0</v>
-      </c>
-      <c r="T34" s="4"/>
+      <c r="Q34" s="1">
+        <v>0</v>
+      </c>
+      <c r="R34" s="1">
+        <v>0</v>
+      </c>
+      <c r="S34" s="1">
+        <v>0</v>
+      </c>
+      <c r="T34" s="1">
+        <v>0</v>
+      </c>
       <c r="U34" s="1" t="s">
         <v>29</v>
       </c>
@@ -4243,19 +4265,19 @@
         <v>0</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="C35" t="s">
-        <v>167</v>
+        <v>101</v>
       </c>
       <c r="D35" t="s">
-        <v>163</v>
+        <v>102</v>
       </c>
       <c r="E35" t="s">
         <v>59</v>
       </c>
       <c r="F35" t="s">
-        <v>163</v>
+        <v>102</v>
       </c>
       <c r="G35" t="b">
         <v>0</v>
@@ -4275,8 +4297,8 @@
       <c r="L35">
         <v>200</v>
       </c>
-      <c r="M35" t="s">
-        <v>164</v>
+      <c r="M35" s="2" t="s">
+        <v>94</v>
       </c>
       <c r="N35" t="b">
         <v>1</v>
@@ -4303,128 +4325,128 @@
         <v>29</v>
       </c>
     </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:21" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="b">
         <v>0</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="C36" t="s">
-        <v>181</v>
-      </c>
-      <c r="D36" t="s">
-        <v>177</v>
-      </c>
-      <c r="E36" t="s">
-        <v>69</v>
-      </c>
-      <c r="F36" t="s">
-        <v>177</v>
-      </c>
-      <c r="G36" t="b">
-        <v>0</v>
-      </c>
-      <c r="H36" t="b">
-        <v>0</v>
-      </c>
-      <c r="I36" t="b">
-        <v>0</v>
-      </c>
-      <c r="J36" t="b">
-        <v>1</v>
-      </c>
-      <c r="K36">
-        <v>1</v>
-      </c>
-      <c r="L36">
-        <v>200</v>
-      </c>
-      <c r="M36" t="s">
-        <v>29</v>
-      </c>
-      <c r="N36" t="b">
-        <v>0</v>
-      </c>
-      <c r="O36">
-        <v>4000</v>
-      </c>
-      <c r="P36" s="1" t="s">
+      <c r="C36" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G36" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H36" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I36" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J36" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="K36" s="2">
+        <v>1</v>
+      </c>
+      <c r="L36" s="2">
+        <v>200</v>
+      </c>
+      <c r="M36" s="2"/>
+      <c r="N36" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="O36" s="2">
+        <v>200</v>
+      </c>
+      <c r="P36" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="Q36" s="1">
-        <v>0</v>
-      </c>
-      <c r="R36" s="1">
-        <v>0</v>
-      </c>
-      <c r="S36" s="1">
-        <v>0</v>
-      </c>
-      <c r="T36" s="1">
-        <v>0</v>
-      </c>
+      <c r="Q36" s="4">
+        <v>0</v>
+      </c>
+      <c r="R36" s="4">
+        <v>0</v>
+      </c>
+      <c r="S36" s="4">
+        <v>0</v>
+      </c>
+      <c r="T36" s="4"/>
       <c r="U36" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="37" spans="1:21" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="b">
         <v>0</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G37" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="H37" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="I37" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="J37" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="K37" s="2">
-        <v>1</v>
-      </c>
-      <c r="L37" s="2">
-        <v>200</v>
-      </c>
-      <c r="M37" s="2"/>
-      <c r="N37" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="O37" s="2">
-        <v>200</v>
-      </c>
-      <c r="P37" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C37" t="s">
+        <v>167</v>
+      </c>
+      <c r="D37" t="s">
+        <v>163</v>
+      </c>
+      <c r="E37" t="s">
+        <v>59</v>
+      </c>
+      <c r="F37" t="s">
+        <v>163</v>
+      </c>
+      <c r="G37" t="b">
+        <v>0</v>
+      </c>
+      <c r="H37" t="b">
+        <v>0</v>
+      </c>
+      <c r="I37" t="b">
+        <v>0</v>
+      </c>
+      <c r="J37" t="b">
+        <v>1</v>
+      </c>
+      <c r="K37">
+        <v>1</v>
+      </c>
+      <c r="L37">
+        <v>200</v>
+      </c>
+      <c r="M37" t="s">
+        <v>164</v>
+      </c>
+      <c r="N37" t="b">
+        <v>1</v>
+      </c>
+      <c r="O37">
+        <v>202</v>
+      </c>
+      <c r="P37" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="Q37" s="4">
-        <v>0</v>
-      </c>
-      <c r="R37" s="4">
-        <v>0</v>
-      </c>
-      <c r="S37" s="4">
-        <v>0</v>
-      </c>
-      <c r="T37" s="4"/>
+      <c r="Q37" s="1">
+        <v>0</v>
+      </c>
+      <c r="R37" s="1">
+        <v>-100000000</v>
+      </c>
+      <c r="S37" s="1">
+        <v>100000000</v>
+      </c>
+      <c r="T37" s="1">
+        <v>0</v>
+      </c>
       <c r="U37" s="1" t="s">
         <v>29</v>
       </c>
@@ -4434,19 +4456,19 @@
         <v>0</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C38" t="s">
-        <v>105</v>
+        <v>181</v>
       </c>
       <c r="D38" t="s">
-        <v>123</v>
+        <v>177</v>
       </c>
       <c r="E38" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="F38" t="s">
-        <v>123</v>
+        <v>177</v>
       </c>
       <c r="G38" t="b">
         <v>0</v>
@@ -4466,14 +4488,14 @@
       <c r="L38">
         <v>200</v>
       </c>
-      <c r="M38" s="2" t="s">
-        <v>105</v>
+      <c r="M38" t="s">
+        <v>29</v>
       </c>
       <c r="N38" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O38">
-        <v>202</v>
+        <v>4000</v>
       </c>
       <c r="P38" s="1" t="s">
         <v>30</v>
@@ -4482,10 +4504,10 @@
         <v>0</v>
       </c>
       <c r="R38" s="1">
-        <v>-100000000</v>
+        <v>0</v>
       </c>
       <c r="S38" s="1">
-        <v>100000000</v>
+        <v>0</v>
       </c>
       <c r="T38" s="1">
         <v>0</v>
@@ -4494,69 +4516,65 @@
         <v>29</v>
       </c>
     </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:21" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="b">
         <v>0</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="C39" t="s">
-        <v>107</v>
-      </c>
-      <c r="D39" t="s">
-        <v>112</v>
-      </c>
-      <c r="E39" t="s">
-        <v>60</v>
-      </c>
-      <c r="F39" t="s">
-        <v>112</v>
-      </c>
-      <c r="G39" t="b">
-        <v>0</v>
-      </c>
-      <c r="H39" t="b">
-        <v>0</v>
-      </c>
-      <c r="I39" t="b">
-        <v>0</v>
-      </c>
-      <c r="J39" t="b">
-        <v>1</v>
-      </c>
-      <c r="K39">
-        <v>1</v>
-      </c>
-      <c r="L39">
-        <v>200</v>
-      </c>
-      <c r="M39" t="s">
-        <v>56</v>
-      </c>
-      <c r="N39" t="b">
-        <v>1</v>
-      </c>
-      <c r="O39">
-        <v>203</v>
-      </c>
-      <c r="P39" s="1" t="s">
+      <c r="C39" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G39" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H39" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I39" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J39" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="K39" s="2">
+        <v>1</v>
+      </c>
+      <c r="L39" s="2">
+        <v>200</v>
+      </c>
+      <c r="M39" s="2"/>
+      <c r="N39" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="O39" s="2">
+        <v>200</v>
+      </c>
+      <c r="P39" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="Q39" s="1">
-        <v>0</v>
-      </c>
-      <c r="R39" s="1">
-        <v>-100000000</v>
-      </c>
-      <c r="S39" s="1">
-        <v>100000000</v>
-      </c>
-      <c r="T39" s="1">
-        <v>0</v>
-      </c>
-      <c r="U39" t="s">
-        <v>117</v>
+      <c r="Q39" s="4">
+        <v>0</v>
+      </c>
+      <c r="R39" s="4">
+        <v>0</v>
+      </c>
+      <c r="S39" s="4">
+        <v>0</v>
+      </c>
+      <c r="T39" s="4"/>
+      <c r="U39" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.3">
@@ -4567,16 +4585,16 @@
         <v>106</v>
       </c>
       <c r="C40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D40" t="s">
-        <v>113</v>
+        <v>123</v>
       </c>
       <c r="E40" t="s">
-        <v>1</v>
+        <v>59</v>
       </c>
       <c r="F40" t="s">
-        <v>113</v>
+        <v>123</v>
       </c>
       <c r="G40" t="b">
         <v>0</v>
@@ -4596,14 +4614,14 @@
       <c r="L40">
         <v>200</v>
       </c>
-      <c r="M40" t="s">
-        <v>29</v>
+      <c r="M40" s="2" t="s">
+        <v>105</v>
       </c>
       <c r="N40" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O40">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="P40" s="1" t="s">
         <v>30</v>
@@ -4612,10 +4630,10 @@
         <v>0</v>
       </c>
       <c r="R40" s="1">
-        <v>0</v>
+        <v>-100000000</v>
       </c>
       <c r="S40" s="1">
-        <v>0</v>
+        <v>100000000</v>
       </c>
       <c r="T40" s="1">
         <v>0</v>
@@ -4632,16 +4650,16 @@
         <v>106</v>
       </c>
       <c r="C41" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D41" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E41" t="s">
-        <v>1</v>
+        <v>60</v>
       </c>
       <c r="F41" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G41" t="b">
         <v>0</v>
@@ -4662,13 +4680,13 @@
         <v>200</v>
       </c>
       <c r="M41" t="s">
-        <v>29</v>
+        <v>56</v>
       </c>
       <c r="N41" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O41">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="P41" s="1" t="s">
         <v>30</v>
@@ -4677,16 +4695,16 @@
         <v>0</v>
       </c>
       <c r="R41" s="1">
-        <v>0</v>
+        <v>-100000000</v>
       </c>
       <c r="S41" s="1">
-        <v>0</v>
+        <v>100000000</v>
       </c>
       <c r="T41" s="1">
         <v>0</v>
       </c>
-      <c r="U41" s="1" t="s">
-        <v>29</v>
+      <c r="U41" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.3">
@@ -4697,16 +4715,16 @@
         <v>106</v>
       </c>
       <c r="C42" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D42" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E42" t="s">
         <v>1</v>
       </c>
       <c r="F42" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G42" t="b">
         <v>0</v>
@@ -4733,7 +4751,7 @@
         <v>0</v>
       </c>
       <c r="O42">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="P42" s="1" t="s">
         <v>30</v>
@@ -4762,16 +4780,16 @@
         <v>106</v>
       </c>
       <c r="C43" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D43" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E43" t="s">
         <v>1</v>
       </c>
       <c r="F43" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="G43" t="b">
         <v>0</v>
@@ -4798,7 +4816,7 @@
         <v>0</v>
       </c>
       <c r="O43">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="P43" s="1" t="s">
         <v>30</v>
@@ -4823,33 +4841,39 @@
       <c r="A44" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="B44" t="s">
-        <v>130</v>
+      <c r="B44" s="2" t="s">
+        <v>106</v>
       </c>
       <c r="C44" t="s">
-        <v>93</v>
+        <v>110</v>
       </c>
       <c r="D44" t="s">
-        <v>12</v>
+        <v>115</v>
       </c>
       <c r="E44" t="s">
         <v>1</v>
       </c>
       <c r="F44" t="s">
-        <v>140</v>
+        <v>115</v>
       </c>
       <c r="G44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J44" t="b">
         <v>1</v>
       </c>
+      <c r="K44">
+        <v>1</v>
+      </c>
+      <c r="L44">
+        <v>200</v>
+      </c>
       <c r="M44" t="s">
         <v>29</v>
       </c>
@@ -4857,19 +4881,22 @@
         <v>0</v>
       </c>
       <c r="O44">
-        <v>100</v>
-      </c>
-      <c r="P44" t="s">
+        <v>202</v>
+      </c>
+      <c r="P44" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="R44" t="s">
-        <v>29</v>
-      </c>
-      <c r="S44" t="b">
-        <v>0</v>
-      </c>
-      <c r="T44">
-        <v>-1</v>
+      <c r="Q44" s="1">
+        <v>0</v>
+      </c>
+      <c r="R44" s="1">
+        <v>0</v>
+      </c>
+      <c r="S44" s="1">
+        <v>0</v>
+      </c>
+      <c r="T44" s="1">
+        <v>0</v>
       </c>
       <c r="U44" s="1" t="s">
         <v>29</v>
@@ -4879,20 +4906,20 @@
       <c r="A45" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="B45" t="s">
-        <v>130</v>
+      <c r="B45" s="2" t="s">
+        <v>106</v>
       </c>
       <c r="C45" t="s">
-        <v>167</v>
+        <v>111</v>
       </c>
       <c r="D45" t="s">
-        <v>163</v>
+        <v>116</v>
       </c>
       <c r="E45" t="s">
-        <v>59</v>
+        <v>1</v>
       </c>
       <c r="F45" t="s">
-        <v>163</v>
+        <v>116</v>
       </c>
       <c r="G45" t="b">
         <v>0</v>
@@ -4913,13 +4940,13 @@
         <v>200</v>
       </c>
       <c r="M45" t="s">
-        <v>164</v>
+        <v>29</v>
       </c>
       <c r="N45" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O45">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="P45" s="1" t="s">
         <v>30</v>
@@ -4928,10 +4955,10 @@
         <v>0</v>
       </c>
       <c r="R45" s="1">
-        <v>-100000000</v>
+        <v>0</v>
       </c>
       <c r="S45" s="1">
-        <v>100000000</v>
+        <v>0</v>
       </c>
       <c r="T45" s="1">
         <v>0</v>
@@ -4945,7 +4972,7 @@
         <v>0</v>
       </c>
       <c r="B46" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="C46" t="s">
         <v>93</v>
@@ -5001,25 +5028,25 @@
         <v>0</v>
       </c>
       <c r="B47" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="C47" t="s">
-        <v>130</v>
+        <v>167</v>
       </c>
       <c r="D47" t="s">
-        <v>129</v>
+        <v>163</v>
       </c>
       <c r="E47" t="s">
         <v>59</v>
       </c>
       <c r="F47" t="s">
-        <v>141</v>
+        <v>163</v>
       </c>
       <c r="G47" t="b">
         <v>0</v>
       </c>
       <c r="H47" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I47" t="b">
         <v>0</v>
@@ -5027,23 +5054,35 @@
       <c r="J47" t="b">
         <v>1</v>
       </c>
+      <c r="K47">
+        <v>1</v>
+      </c>
+      <c r="L47">
+        <v>200</v>
+      </c>
       <c r="M47" t="s">
-        <v>130</v>
+        <v>164</v>
       </c>
       <c r="N47" t="b">
         <v>1</v>
       </c>
       <c r="O47">
-        <v>-1</v>
-      </c>
-      <c r="R47" t="s">
-        <v>29</v>
-      </c>
-      <c r="S47" t="b">
-        <v>0</v>
-      </c>
-      <c r="T47">
-        <v>-1</v>
+        <v>202</v>
+      </c>
+      <c r="P47" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q47" s="1">
+        <v>0</v>
+      </c>
+      <c r="R47" s="1">
+        <v>-100000000</v>
+      </c>
+      <c r="S47" s="1">
+        <v>100000000</v>
+      </c>
+      <c r="T47" s="1">
+        <v>0</v>
       </c>
       <c r="U47" s="1" t="s">
         <v>29</v>
@@ -5057,35 +5096,29 @@
         <v>137</v>
       </c>
       <c r="C48" t="s">
-        <v>181</v>
+        <v>93</v>
       </c>
       <c r="D48" t="s">
-        <v>177</v>
+        <v>12</v>
       </c>
       <c r="E48" t="s">
-        <v>69</v>
+        <v>1</v>
       </c>
       <c r="F48" t="s">
-        <v>177</v>
+        <v>140</v>
       </c>
       <c r="G48" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H48" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I48" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J48" t="b">
         <v>1</v>
       </c>
-      <c r="K48">
-        <v>1</v>
-      </c>
-      <c r="L48">
-        <v>200</v>
-      </c>
       <c r="M48" t="s">
         <v>29</v>
       </c>
@@ -5093,22 +5126,19 @@
         <v>0</v>
       </c>
       <c r="O48">
-        <v>4000</v>
-      </c>
-      <c r="P48" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="P48" t="s">
         <v>30</v>
       </c>
-      <c r="Q48" s="1">
-        <v>0</v>
-      </c>
-      <c r="R48" s="1">
-        <v>0</v>
-      </c>
-      <c r="S48" s="1">
-        <v>0</v>
-      </c>
-      <c r="T48" s="1">
-        <v>0</v>
+      <c r="R48" t="s">
+        <v>29</v>
+      </c>
+      <c r="S48" t="b">
+        <v>0</v>
+      </c>
+      <c r="T48">
+        <v>-1</v>
       </c>
       <c r="U48" s="1" t="s">
         <v>29</v>
@@ -5119,43 +5149,40 @@
         <v>0</v>
       </c>
       <c r="B49" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="C49" t="s">
-        <v>109</v>
+        <v>130</v>
       </c>
       <c r="D49" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="E49" t="s">
-        <v>1</v>
+        <v>59</v>
       </c>
       <c r="F49" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="G49" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H49" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I49" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J49" t="b">
         <v>1</v>
       </c>
       <c r="M49" t="s">
-        <v>29</v>
+        <v>130</v>
       </c>
       <c r="N49" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O49">
-        <v>100</v>
-      </c>
-      <c r="P49" t="s">
-        <v>30</v>
+        <v>-1</v>
       </c>
       <c r="R49" t="s">
         <v>29</v>
@@ -5175,25 +5202,25 @@
         <v>0</v>
       </c>
       <c r="B50" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="C50" t="s">
-        <v>137</v>
+        <v>181</v>
       </c>
       <c r="D50" t="s">
-        <v>136</v>
+        <v>177</v>
       </c>
       <c r="E50" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="F50" t="s">
-        <v>144</v>
+        <v>177</v>
       </c>
       <c r="G50" t="b">
         <v>0</v>
       </c>
       <c r="H50" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I50" t="b">
         <v>0</v>
@@ -5201,23 +5228,35 @@
       <c r="J50" t="b">
         <v>1</v>
       </c>
+      <c r="K50">
+        <v>1</v>
+      </c>
+      <c r="L50">
+        <v>200</v>
+      </c>
       <c r="M50" t="s">
-        <v>137</v>
+        <v>29</v>
       </c>
       <c r="N50" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O50">
-        <v>-1</v>
-      </c>
-      <c r="R50" t="s">
-        <v>29</v>
-      </c>
-      <c r="S50" t="b">
-        <v>0</v>
-      </c>
-      <c r="T50">
-        <v>-1</v>
+        <v>4000</v>
+      </c>
+      <c r="P50" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q50" s="1">
+        <v>0</v>
+      </c>
+      <c r="R50" s="1">
+        <v>0</v>
+      </c>
+      <c r="S50" s="1">
+        <v>0</v>
+      </c>
+      <c r="T50" s="1">
+        <v>0</v>
       </c>
       <c r="U50" s="1" t="s">
         <v>29</v>
@@ -5231,19 +5270,22 @@
         <v>134</v>
       </c>
       <c r="C51" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="D51" t="s">
-        <v>112</v>
+        <v>142</v>
       </c>
       <c r="E51" t="s">
-        <v>60</v>
+        <v>1</v>
+      </c>
+      <c r="F51" t="s">
+        <v>143</v>
       </c>
       <c r="G51" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H51" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I51" t="b">
         <v>1</v>
@@ -5258,7 +5300,10 @@
         <v>0</v>
       </c>
       <c r="O51">
-        <v>-1</v>
+        <v>100</v>
+      </c>
+      <c r="P51" t="s">
+        <v>30</v>
       </c>
       <c r="R51" t="s">
         <v>29</v>
@@ -5269,8 +5314,8 @@
       <c r="T51">
         <v>-1</v>
       </c>
-      <c r="U51" t="s">
-        <v>146</v>
+      <c r="U51" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="52" spans="1:21" x14ac:dyDescent="0.3">
@@ -5281,37 +5326,37 @@
         <v>134</v>
       </c>
       <c r="C52" t="s">
-        <v>110</v>
+        <v>137</v>
       </c>
       <c r="D52" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
       <c r="E52" t="s">
-        <v>1</v>
+        <v>59</v>
+      </c>
+      <c r="F52" t="s">
+        <v>144</v>
       </c>
       <c r="G52" t="b">
         <v>0</v>
       </c>
       <c r="H52" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I52" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J52" t="b">
         <v>1</v>
       </c>
       <c r="M52" t="s">
-        <v>29</v>
+        <v>137</v>
       </c>
       <c r="N52" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O52">
-        <v>200</v>
-      </c>
-      <c r="P52" t="s">
-        <v>30</v>
+        <v>-1</v>
       </c>
       <c r="R52" t="s">
         <v>29</v>
@@ -5322,8 +5367,8 @@
       <c r="T52">
         <v>-1</v>
       </c>
-      <c r="U52">
-        <v>-1</v>
+      <c r="U52" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="53" spans="1:21" x14ac:dyDescent="0.3">
@@ -5334,19 +5379,19 @@
         <v>134</v>
       </c>
       <c r="C53" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D53" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E53" t="s">
-        <v>1</v>
+        <v>60</v>
       </c>
       <c r="G53" t="b">
         <v>0</v>
       </c>
       <c r="H53" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I53" t="b">
         <v>1</v>
@@ -5361,10 +5406,7 @@
         <v>0</v>
       </c>
       <c r="O53">
-        <v>200</v>
-      </c>
-      <c r="P53" t="s">
-        <v>30</v>
+        <v>-1</v>
       </c>
       <c r="R53" t="s">
         <v>29</v>
@@ -5375,8 +5417,8 @@
       <c r="T53">
         <v>-1</v>
       </c>
-      <c r="U53">
-        <v>-1</v>
+      <c r="U53" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="54" spans="1:21" x14ac:dyDescent="0.3">
@@ -5387,10 +5429,10 @@
         <v>134</v>
       </c>
       <c r="C54" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D54" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E54" t="s">
         <v>1</v>
@@ -5414,7 +5456,7 @@
         <v>0</v>
       </c>
       <c r="O54">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="P54" t="s">
         <v>30</v>
@@ -5437,25 +5479,22 @@
         <v>0</v>
       </c>
       <c r="B55" t="s">
-        <v>150</v>
+        <v>134</v>
       </c>
       <c r="C55" t="s">
-        <v>93</v>
+        <v>108</v>
       </c>
       <c r="D55" t="s">
-        <v>12</v>
+        <v>113</v>
       </c>
       <c r="E55" t="s">
         <v>1</v>
       </c>
-      <c r="F55" t="s">
-        <v>162</v>
-      </c>
       <c r="G55" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H55" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I55" t="b">
         <v>1</v>
@@ -5470,7 +5509,7 @@
         <v>0</v>
       </c>
       <c r="O55">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="P55" t="s">
         <v>30</v>
@@ -5493,40 +5532,40 @@
         <v>0</v>
       </c>
       <c r="B56" t="s">
+        <v>134</v>
+      </c>
+      <c r="C56" t="s">
+        <v>111</v>
+      </c>
+      <c r="D56" t="s">
+        <v>148</v>
+      </c>
+      <c r="E56" t="s">
+        <v>1</v>
+      </c>
+      <c r="G56" t="b">
+        <v>0</v>
+      </c>
+      <c r="H56" t="b">
+        <v>0</v>
+      </c>
+      <c r="I56" t="b">
+        <v>1</v>
+      </c>
+      <c r="J56" t="b">
+        <v>1</v>
+      </c>
+      <c r="M56" t="s">
+        <v>29</v>
+      </c>
+      <c r="N56" t="b">
+        <v>0</v>
+      </c>
+      <c r="O56">
         <v>150</v>
       </c>
-      <c r="C56" t="s">
-        <v>157</v>
-      </c>
-      <c r="D56" t="s">
-        <v>158</v>
-      </c>
-      <c r="E56" t="s">
-        <v>59</v>
-      </c>
-      <c r="F56" t="s">
-        <v>159</v>
-      </c>
-      <c r="G56" t="b">
-        <v>0</v>
-      </c>
-      <c r="H56" t="b">
-        <v>0</v>
-      </c>
-      <c r="I56" t="b">
-        <v>0</v>
-      </c>
-      <c r="J56" t="b">
-        <v>1</v>
-      </c>
-      <c r="M56" t="s">
-        <v>150</v>
-      </c>
-      <c r="N56" t="b">
-        <v>1</v>
-      </c>
-      <c r="O56">
-        <v>-1</v>
+      <c r="P56" t="s">
+        <v>30</v>
       </c>
       <c r="R56" t="s">
         <v>29</v>
@@ -5549,37 +5588,40 @@
         <v>150</v>
       </c>
       <c r="C57" t="s">
-        <v>160</v>
+        <v>93</v>
       </c>
       <c r="D57" t="s">
-        <v>153</v>
+        <v>12</v>
       </c>
       <c r="E57" t="s">
-        <v>59</v>
+        <v>1</v>
       </c>
       <c r="F57" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="G57" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H57" t="b">
         <v>1</v>
       </c>
       <c r="I57" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J57" t="b">
         <v>1</v>
       </c>
       <c r="M57" t="s">
-        <v>154</v>
+        <v>29</v>
       </c>
       <c r="N57" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O57">
-        <v>-1</v>
+        <v>100</v>
+      </c>
+      <c r="P57" t="s">
+        <v>30</v>
       </c>
       <c r="R57" t="s">
         <v>29</v>
@@ -5599,43 +5641,40 @@
         <v>0</v>
       </c>
       <c r="B58" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C58" t="s">
-        <v>93</v>
+        <v>157</v>
       </c>
       <c r="D58" t="s">
-        <v>12</v>
+        <v>158</v>
       </c>
       <c r="E58" t="s">
-        <v>1</v>
+        <v>59</v>
       </c>
       <c r="F58" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="G58" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H58" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I58" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J58" t="b">
         <v>1</v>
       </c>
       <c r="M58" t="s">
-        <v>29</v>
+        <v>150</v>
       </c>
       <c r="N58" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O58">
-        <v>100</v>
-      </c>
-      <c r="P58" t="s">
-        <v>30</v>
+        <v>-1</v>
       </c>
       <c r="R58" t="s">
         <v>29</v>
@@ -5655,43 +5694,40 @@
         <v>0</v>
       </c>
       <c r="B59" t="s">
-        <v>164</v>
+        <v>150</v>
       </c>
       <c r="C59" t="s">
-        <v>93</v>
+        <v>160</v>
       </c>
       <c r="D59" t="s">
-        <v>12</v>
+        <v>153</v>
       </c>
       <c r="E59" t="s">
-        <v>1</v>
+        <v>59</v>
       </c>
       <c r="F59" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G59" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H59" t="b">
         <v>1</v>
       </c>
       <c r="I59" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J59" t="b">
         <v>1</v>
       </c>
       <c r="M59" t="s">
-        <v>29</v>
+        <v>154</v>
       </c>
       <c r="N59" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O59">
-        <v>100</v>
-      </c>
-      <c r="P59" t="s">
-        <v>30</v>
+        <v>-1</v>
       </c>
       <c r="R59" t="s">
         <v>29</v>
@@ -5711,7 +5747,7 @@
         <v>0</v>
       </c>
       <c r="B60" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
       <c r="C60" t="s">
         <v>93</v>
@@ -5767,28 +5803,28 @@
         <v>0</v>
       </c>
       <c r="B61" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C61" t="s">
-        <v>167</v>
+        <v>93</v>
       </c>
       <c r="D61" t="s">
-        <v>163</v>
+        <v>12</v>
       </c>
       <c r="E61" t="s">
-        <v>59</v>
+        <v>1</v>
       </c>
       <c r="F61" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G61" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H61" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I61" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J61" t="b">
         <v>1</v>
@@ -5800,31 +5836,28 @@
         <v>200</v>
       </c>
       <c r="M61" t="s">
-        <v>164</v>
+        <v>29</v>
       </c>
       <c r="N61" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O61">
-        <v>202</v>
-      </c>
-      <c r="P61" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="P61" t="s">
         <v>30</v>
       </c>
-      <c r="Q61" s="1">
-        <v>0</v>
-      </c>
-      <c r="R61" s="1">
-        <v>-100000000</v>
-      </c>
-      <c r="S61" s="1">
-        <v>100000000</v>
-      </c>
-      <c r="T61" s="1">
-        <v>0</v>
-      </c>
-      <c r="U61" s="1" t="s">
-        <v>29</v>
+      <c r="R61" t="s">
+        <v>29</v>
+      </c>
+      <c r="S61" t="b">
+        <v>0</v>
+      </c>
+      <c r="T61">
+        <v>-1</v>
+      </c>
+      <c r="U61">
+        <v>-1</v>
       </c>
     </row>
     <row r="62" spans="1:21" x14ac:dyDescent="0.3">
@@ -5832,19 +5865,19 @@
         <v>0</v>
       </c>
       <c r="B62" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C62" t="s">
-        <v>180</v>
+        <v>210</v>
       </c>
       <c r="D62" t="s">
-        <v>87</v>
+        <v>211</v>
       </c>
       <c r="E62" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="F62" t="s">
-        <v>87</v>
+        <v>211</v>
       </c>
       <c r="G62" t="b">
         <v>0</v>
@@ -5859,19 +5892,19 @@
         <v>1</v>
       </c>
       <c r="K62">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L62">
         <v>200</v>
       </c>
-      <c r="M62" t="s">
-        <v>29</v>
+      <c r="M62" s="2" t="s">
+        <v>95</v>
       </c>
       <c r="N62" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O62">
-        <v>4000</v>
+        <v>202</v>
       </c>
       <c r="P62" s="1" t="s">
         <v>30</v>
@@ -5880,10 +5913,10 @@
         <v>0</v>
       </c>
       <c r="R62" s="1">
-        <v>0</v>
+        <v>-100000000</v>
       </c>
       <c r="S62" s="1">
-        <v>0</v>
+        <v>100000000</v>
       </c>
       <c r="T62" s="1">
         <v>0</v>
@@ -5897,7 +5930,7 @@
         <v>0</v>
       </c>
       <c r="B63" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C63" t="s">
         <v>93</v>
@@ -5953,7 +5986,7 @@
         <v>0</v>
       </c>
       <c r="B64" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C64" t="s">
         <v>167</v>
@@ -6018,19 +6051,19 @@
         <v>0</v>
       </c>
       <c r="B65" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C65" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D65" t="s">
-        <v>177</v>
+        <v>87</v>
       </c>
       <c r="E65" t="s">
         <v>69</v>
       </c>
       <c r="F65" t="s">
-        <v>177</v>
+        <v>87</v>
       </c>
       <c r="G65" t="b">
         <v>0</v>
@@ -6083,7 +6116,7 @@
         <v>0</v>
       </c>
       <c r="B66" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="C66" t="s">
         <v>93</v>
@@ -6139,55 +6172,64 @@
         <v>0</v>
       </c>
       <c r="B67" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="C67" t="s">
-        <v>206</v>
+        <v>167</v>
       </c>
       <c r="D67" t="s">
-        <v>12</v>
+        <v>163</v>
       </c>
       <c r="E67" t="s">
-        <v>1</v>
+        <v>59</v>
       </c>
       <c r="F67" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="G67" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H67" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I67" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J67" t="b">
         <v>1</v>
       </c>
+      <c r="K67">
+        <v>1</v>
+      </c>
+      <c r="L67">
+        <v>200</v>
+      </c>
       <c r="M67" t="s">
-        <v>29</v>
+        <v>164</v>
       </c>
       <c r="N67" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O67">
-        <v>100</v>
-      </c>
-      <c r="P67" t="s">
+        <v>202</v>
+      </c>
+      <c r="P67" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="R67" t="s">
-        <v>29</v>
-      </c>
-      <c r="S67" t="b">
-        <v>0</v>
-      </c>
-      <c r="T67">
-        <v>-1</v>
-      </c>
-      <c r="U67">
-        <v>-1</v>
+      <c r="Q67" s="1">
+        <v>0</v>
+      </c>
+      <c r="R67" s="1">
+        <v>-100000000</v>
+      </c>
+      <c r="S67" s="1">
+        <v>100000000</v>
+      </c>
+      <c r="T67" s="1">
+        <v>0</v>
+      </c>
+      <c r="U67" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="68" spans="1:21" x14ac:dyDescent="0.3">
@@ -6195,32 +6237,38 @@
         <v>0</v>
       </c>
       <c r="B68" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="C68" t="s">
-        <v>93</v>
+        <v>181</v>
       </c>
       <c r="D68" t="s">
-        <v>12</v>
+        <v>177</v>
       </c>
       <c r="E68" t="s">
-        <v>1</v>
+        <v>69</v>
       </c>
       <c r="F68" t="s">
-        <v>162</v>
+        <v>177</v>
       </c>
       <c r="G68" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H68" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I68" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J68" t="b">
         <v>1</v>
       </c>
+      <c r="K68">
+        <v>1</v>
+      </c>
+      <c r="L68">
+        <v>200</v>
+      </c>
       <c r="M68" t="s">
         <v>29</v>
       </c>
@@ -6228,22 +6276,25 @@
         <v>0</v>
       </c>
       <c r="O68">
-        <v>100</v>
-      </c>
-      <c r="P68" t="s">
+        <v>4000</v>
+      </c>
+      <c r="P68" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="R68" t="s">
-        <v>29</v>
-      </c>
-      <c r="S68" t="b">
-        <v>0</v>
-      </c>
-      <c r="T68">
-        <v>-1</v>
-      </c>
-      <c r="U68">
-        <v>-1</v>
+      <c r="Q68" s="1">
+        <v>0</v>
+      </c>
+      <c r="R68" s="1">
+        <v>0</v>
+      </c>
+      <c r="S68" s="1">
+        <v>0</v>
+      </c>
+      <c r="T68" s="1">
+        <v>0</v>
+      </c>
+      <c r="U68" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="69" spans="1:21" x14ac:dyDescent="0.3">
@@ -6251,7 +6302,7 @@
         <v>0</v>
       </c>
       <c r="B69" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C69" t="s">
         <v>93</v>
@@ -6307,10 +6358,10 @@
         <v>0</v>
       </c>
       <c r="B70" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C70" t="s">
-        <v>93</v>
+        <v>206</v>
       </c>
       <c r="D70" t="s">
         <v>12</v>
@@ -6363,7 +6414,7 @@
         <v>0</v>
       </c>
       <c r="B71" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C71" t="s">
         <v>93</v>
@@ -6419,7 +6470,7 @@
         <v>0</v>
       </c>
       <c r="B72" t="s">
-        <v>200</v>
+        <v>185</v>
       </c>
       <c r="C72" t="s">
         <v>93</v>
@@ -6452,7 +6503,7 @@
         <v>0</v>
       </c>
       <c r="O72">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="P72" t="s">
         <v>30</v>
@@ -6475,64 +6526,55 @@
         <v>0</v>
       </c>
       <c r="B73" t="s">
-        <v>154</v>
+        <v>186</v>
       </c>
       <c r="C73" t="s">
-        <v>167</v>
+        <v>93</v>
       </c>
       <c r="D73" t="s">
-        <v>163</v>
+        <v>12</v>
       </c>
       <c r="E73" t="s">
-        <v>59</v>
+        <v>1</v>
       </c>
       <c r="F73" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G73" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H73" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I73" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J73" t="b">
         <v>1</v>
       </c>
-      <c r="K73">
-        <v>1</v>
-      </c>
-      <c r="L73">
-        <v>200</v>
-      </c>
       <c r="M73" t="s">
-        <v>164</v>
+        <v>29</v>
       </c>
       <c r="N73" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O73">
-        <v>202</v>
-      </c>
-      <c r="P73" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="P73" t="s">
         <v>30</v>
       </c>
-      <c r="Q73" s="1">
-        <v>0</v>
-      </c>
-      <c r="R73" s="1">
-        <v>-100000000</v>
-      </c>
-      <c r="S73" s="1">
-        <v>100000000</v>
-      </c>
-      <c r="T73" s="1">
-        <v>0</v>
-      </c>
-      <c r="U73" s="1" t="s">
-        <v>29</v>
+      <c r="R73" t="s">
+        <v>29</v>
+      </c>
+      <c r="S73" t="b">
+        <v>0</v>
+      </c>
+      <c r="T73">
+        <v>-1</v>
+      </c>
+      <c r="U73">
+        <v>-1</v>
       </c>
     </row>
     <row r="74" spans="1:21" x14ac:dyDescent="0.3">
@@ -6540,64 +6582,55 @@
         <v>0</v>
       </c>
       <c r="B74" t="s">
-        <v>96</v>
+        <v>187</v>
       </c>
       <c r="C74" t="s">
-        <v>167</v>
+        <v>93</v>
       </c>
       <c r="D74" t="s">
-        <v>163</v>
+        <v>12</v>
       </c>
       <c r="E74" t="s">
-        <v>59</v>
+        <v>1</v>
       </c>
       <c r="F74" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G74" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H74" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I74" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J74" t="b">
         <v>1</v>
       </c>
-      <c r="K74">
-        <v>1</v>
-      </c>
-      <c r="L74">
-        <v>200</v>
-      </c>
       <c r="M74" t="s">
-        <v>164</v>
+        <v>29</v>
       </c>
       <c r="N74" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O74">
-        <v>202</v>
-      </c>
-      <c r="P74" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="P74" t="s">
         <v>30</v>
       </c>
-      <c r="Q74" s="1">
-        <v>0</v>
-      </c>
-      <c r="R74" s="1">
-        <v>-100000000</v>
-      </c>
-      <c r="S74" s="1">
-        <v>100000000</v>
-      </c>
-      <c r="T74" s="1">
-        <v>0</v>
-      </c>
-      <c r="U74" s="1" t="s">
-        <v>29</v>
+      <c r="R74" t="s">
+        <v>29</v>
+      </c>
+      <c r="S74" t="b">
+        <v>0</v>
+      </c>
+      <c r="T74">
+        <v>-1</v>
+      </c>
+      <c r="U74">
+        <v>-1</v>
       </c>
     </row>
     <row r="75" spans="1:21" x14ac:dyDescent="0.3">
@@ -6605,64 +6638,55 @@
         <v>0</v>
       </c>
       <c r="B75" t="s">
-        <v>187</v>
+        <v>200</v>
       </c>
       <c r="C75" t="s">
-        <v>167</v>
+        <v>93</v>
       </c>
       <c r="D75" t="s">
-        <v>163</v>
+        <v>12</v>
       </c>
       <c r="E75" t="s">
-        <v>59</v>
+        <v>1</v>
       </c>
       <c r="F75" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G75" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H75" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I75" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J75" t="b">
         <v>1</v>
       </c>
-      <c r="K75">
-        <v>1</v>
-      </c>
-      <c r="L75">
-        <v>200</v>
-      </c>
       <c r="M75" t="s">
-        <v>164</v>
+        <v>29</v>
       </c>
       <c r="N75" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O75">
-        <v>202</v>
-      </c>
-      <c r="P75" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="P75" t="s">
         <v>30</v>
       </c>
-      <c r="Q75" s="1">
-        <v>0</v>
-      </c>
-      <c r="R75" s="1">
-        <v>-100000000</v>
-      </c>
-      <c r="S75" s="1">
-        <v>100000000</v>
-      </c>
-      <c r="T75" s="1">
-        <v>0</v>
-      </c>
-      <c r="U75" s="1" t="s">
-        <v>29</v>
+      <c r="R75" t="s">
+        <v>29</v>
+      </c>
+      <c r="S75" t="b">
+        <v>0</v>
+      </c>
+      <c r="T75">
+        <v>-1</v>
+      </c>
+      <c r="U75">
+        <v>-1</v>
       </c>
     </row>
     <row r="76" spans="1:21" x14ac:dyDescent="0.3">
@@ -6670,7 +6694,7 @@
         <v>0</v>
       </c>
       <c r="B76" t="s">
-        <v>186</v>
+        <v>154</v>
       </c>
       <c r="C76" t="s">
         <v>167</v>
@@ -6735,7 +6759,7 @@
         <v>0</v>
       </c>
       <c r="B77" t="s">
-        <v>185</v>
+        <v>96</v>
       </c>
       <c r="C77" t="s">
         <v>167</v>
@@ -6800,7 +6824,7 @@
         <v>0</v>
       </c>
       <c r="B78" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="C78" t="s">
         <v>167</v>
@@ -6865,7 +6889,7 @@
         <v>0</v>
       </c>
       <c r="B79" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="C79" t="s">
         <v>167</v>
@@ -6930,7 +6954,7 @@
         <v>0</v>
       </c>
       <c r="B80" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="C80" t="s">
         <v>167</v>
@@ -6990,18 +7014,213 @@
         <v>29</v>
       </c>
     </row>
+    <row r="81" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A81" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B81" t="s">
+        <v>184</v>
+      </c>
+      <c r="C81" t="s">
+        <v>167</v>
+      </c>
+      <c r="D81" t="s">
+        <v>163</v>
+      </c>
+      <c r="E81" t="s">
+        <v>59</v>
+      </c>
+      <c r="F81" t="s">
+        <v>163</v>
+      </c>
+      <c r="G81" t="b">
+        <v>0</v>
+      </c>
+      <c r="H81" t="b">
+        <v>0</v>
+      </c>
+      <c r="I81" t="b">
+        <v>0</v>
+      </c>
+      <c r="J81" t="b">
+        <v>1</v>
+      </c>
+      <c r="K81">
+        <v>1</v>
+      </c>
+      <c r="L81">
+        <v>200</v>
+      </c>
+      <c r="M81" t="s">
+        <v>164</v>
+      </c>
+      <c r="N81" t="b">
+        <v>1</v>
+      </c>
+      <c r="O81">
+        <v>202</v>
+      </c>
+      <c r="P81" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q81" s="1">
+        <v>0</v>
+      </c>
+      <c r="R81" s="1">
+        <v>-100000000</v>
+      </c>
+      <c r="S81" s="1">
+        <v>100000000</v>
+      </c>
+      <c r="T81" s="1">
+        <v>0</v>
+      </c>
+      <c r="U81" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="82" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A82" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B82" t="s">
+        <v>183</v>
+      </c>
+      <c r="C82" t="s">
+        <v>167</v>
+      </c>
+      <c r="D82" t="s">
+        <v>163</v>
+      </c>
+      <c r="E82" t="s">
+        <v>59</v>
+      </c>
+      <c r="F82" t="s">
+        <v>163</v>
+      </c>
+      <c r="G82" t="b">
+        <v>0</v>
+      </c>
+      <c r="H82" t="b">
+        <v>0</v>
+      </c>
+      <c r="I82" t="b">
+        <v>0</v>
+      </c>
+      <c r="J82" t="b">
+        <v>1</v>
+      </c>
+      <c r="K82">
+        <v>1</v>
+      </c>
+      <c r="L82">
+        <v>200</v>
+      </c>
+      <c r="M82" t="s">
+        <v>164</v>
+      </c>
+      <c r="N82" t="b">
+        <v>1</v>
+      </c>
+      <c r="O82">
+        <v>202</v>
+      </c>
+      <c r="P82" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q82" s="1">
+        <v>0</v>
+      </c>
+      <c r="R82" s="1">
+        <v>-100000000</v>
+      </c>
+      <c r="S82" s="1">
+        <v>100000000</v>
+      </c>
+      <c r="T82" s="1">
+        <v>0</v>
+      </c>
+      <c r="U82" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="83" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A83" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B83" t="s">
+        <v>182</v>
+      </c>
+      <c r="C83" t="s">
+        <v>167</v>
+      </c>
+      <c r="D83" t="s">
+        <v>163</v>
+      </c>
+      <c r="E83" t="s">
+        <v>59</v>
+      </c>
+      <c r="F83" t="s">
+        <v>163</v>
+      </c>
+      <c r="G83" t="b">
+        <v>0</v>
+      </c>
+      <c r="H83" t="b">
+        <v>0</v>
+      </c>
+      <c r="I83" t="b">
+        <v>0</v>
+      </c>
+      <c r="J83" t="b">
+        <v>1</v>
+      </c>
+      <c r="K83">
+        <v>1</v>
+      </c>
+      <c r="L83">
+        <v>200</v>
+      </c>
+      <c r="M83" t="s">
+        <v>164</v>
+      </c>
+      <c r="N83" t="b">
+        <v>1</v>
+      </c>
+      <c r="O83">
+        <v>202</v>
+      </c>
+      <c r="P83" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q83" s="1">
+        <v>0</v>
+      </c>
+      <c r="R83" s="1">
+        <v>-100000000</v>
+      </c>
+      <c r="S83" s="1">
+        <v>100000000</v>
+      </c>
+      <c r="T83" s="1">
+        <v>0</v>
+      </c>
+      <c r="U83" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E7 E16:E20 E35:E36 E27:E33 E22 E38:E65546">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E7 E16:E20 E37:E38 E40:E65549 E22 E27:E35">
       <formula1>"Boolean,Date,Decimal,Double,Integer,Lookup,Money,Picklist,String,Memo,Status"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P38:P65546 P35:P36 P27:P33 P22 P2:P20">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P2:P20 P37:P38 P40:P65549 P22 P27:P35">
       <formula1>"Text,TextArea,Email,Url,TickerSymbol,Phone"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt=" - " sqref="P37 P34 P21 P23:P26">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt=" - " sqref="P39 P36 P21 P23:P26">
       <formula1>"Text,TextArea,Email,Url,TickerSymbol,Phone"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt=" - " sqref="E37 E34 E21 E23:E26">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt=" - " sqref="E39 E36 E21 E23:E26">
       <formula1>"Boolean,Customer,Date,Decimal,Double,Integer,Lookup,Money,Picklist,String,Memo,Status"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>